<commit_message>
updated timeframe spreadsheet, formatting update on doc
</commit_message>
<xml_diff>
--- a/Assignment 3 timeframe..xlsx
+++ b/Assignment 3 timeframe..xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A1AE83-5964-46B2-B045-9548DBEE6DCF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FDAF2D-29E5-481D-AE1E-6BC67DE76C1C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20052" yWindow="4092" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,12 +26,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="142">
   <si>
     <t>Task 3</t>
   </si>
@@ -405,9 +410,6 @@
     <t>Due Date 19th May</t>
   </si>
   <si>
-    <t>Project Timeframe end date: 22/07/2019</t>
-  </si>
-  <si>
     <t>ASSIGNED</t>
   </si>
   <si>
@@ -444,15 +446,9 @@
     <t>Test Scene feedback with demographics</t>
   </si>
   <si>
-    <t>Main Player character conepts</t>
-  </si>
-  <si>
     <t>Relationship system concepts</t>
   </si>
   <si>
-    <t>early graphic development models/objects</t>
-  </si>
-  <si>
     <t>Sample soundtrack/bgm</t>
   </si>
   <si>
@@ -496,6 +492,18 @@
   </si>
   <si>
     <t>Marketing</t>
+  </si>
+  <si>
+    <t>Music and sound mixing</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
+  </si>
+  <si>
+    <t>Main Player character concepts</t>
+  </si>
+  <si>
+    <t>Early graphic development models/objects</t>
   </si>
 </sst>
 </file>
@@ -698,7 +706,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -837,8 +845,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -998,12 +1012,60 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="hair">
         <color indexed="64"/>
       </left>
-      <right style="slantDashDot">
-        <color rgb="FFC00000"/>
-      </right>
+      <right/>
       <top style="hair">
         <color indexed="64"/>
       </top>
@@ -1013,11 +1075,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashDot">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="0" tint="-0.14996795556505021"/>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1052,7 +1133,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1303,6 +1384,103 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="23" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="12" xfId="11" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="8" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="13" xfId="10" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="13" xfId="11" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="14" xfId="11" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="9" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="13" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -1319,121 +1497,104 @@
     <xf numFmtId="167" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="23" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="15" xfId="9" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="16" xfId="9" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="18" xfId="10" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="17" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="12" xfId="11" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="8" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="13" xfId="10" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="9" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="13" xfId="11" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="17" xfId="11" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="6" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="17" xfId="11" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="17" xfId="11" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="15" xfId="11" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="9" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="13" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="20" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="19" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="19" xfId="11" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -2056,14 +2217,14 @@
       <c r="B3" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="E3" s="97">
+      <c r="D3" s="124"/>
+      <c r="E3" s="122">
         <v>43570</v>
       </c>
-      <c r="F3" s="97"/>
+      <c r="F3" s="122"/>
       <c r="I3">
         <v>1</v>
       </c>
@@ -2075,104 +2236,104 @@
       <c r="B4" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="123" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="89"/>
+      <c r="D4" s="124"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="94">
+      <c r="I4" s="119">
         <f>I5</f>
         <v>43570</v>
       </c>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="95"/>
-      <c r="O4" s="96"/>
-      <c r="P4" s="94">
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="120"/>
+      <c r="O4" s="121"/>
+      <c r="P4" s="119">
         <f>P5</f>
         <v>43577</v>
       </c>
-      <c r="Q4" s="95"/>
-      <c r="R4" s="95"/>
-      <c r="S4" s="95"/>
-      <c r="T4" s="95"/>
-      <c r="U4" s="95"/>
-      <c r="V4" s="96"/>
-      <c r="W4" s="94">
+      <c r="Q4" s="120"/>
+      <c r="R4" s="120"/>
+      <c r="S4" s="120"/>
+      <c r="T4" s="120"/>
+      <c r="U4" s="120"/>
+      <c r="V4" s="121"/>
+      <c r="W4" s="119">
         <f>W5</f>
         <v>43584</v>
       </c>
-      <c r="X4" s="95"/>
-      <c r="Y4" s="95"/>
-      <c r="Z4" s="95"/>
-      <c r="AA4" s="95"/>
-      <c r="AB4" s="95"/>
-      <c r="AC4" s="96"/>
-      <c r="AD4" s="94">
+      <c r="X4" s="120"/>
+      <c r="Y4" s="120"/>
+      <c r="Z4" s="120"/>
+      <c r="AA4" s="120"/>
+      <c r="AB4" s="120"/>
+      <c r="AC4" s="121"/>
+      <c r="AD4" s="119">
         <f>AD5</f>
         <v>43591</v>
       </c>
-      <c r="AE4" s="95"/>
-      <c r="AF4" s="95"/>
-      <c r="AG4" s="95"/>
-      <c r="AH4" s="95"/>
-      <c r="AI4" s="95"/>
-      <c r="AJ4" s="96"/>
-      <c r="AK4" s="91">
+      <c r="AE4" s="120"/>
+      <c r="AF4" s="120"/>
+      <c r="AG4" s="120"/>
+      <c r="AH4" s="120"/>
+      <c r="AI4" s="120"/>
+      <c r="AJ4" s="121"/>
+      <c r="AK4" s="126">
         <f>AK5</f>
         <v>43598</v>
       </c>
-      <c r="AL4" s="92"/>
-      <c r="AM4" s="92"/>
-      <c r="AN4" s="92"/>
-      <c r="AO4" s="92"/>
-      <c r="AP4" s="92"/>
-      <c r="AQ4" s="93"/>
-      <c r="AR4" s="94">
+      <c r="AL4" s="127"/>
+      <c r="AM4" s="127"/>
+      <c r="AN4" s="127"/>
+      <c r="AO4" s="127"/>
+      <c r="AP4" s="127"/>
+      <c r="AQ4" s="128"/>
+      <c r="AR4" s="119">
         <f>AR5</f>
         <v>43605</v>
       </c>
-      <c r="AS4" s="95"/>
-      <c r="AT4" s="95"/>
-      <c r="AU4" s="95"/>
-      <c r="AV4" s="95"/>
-      <c r="AW4" s="95"/>
-      <c r="AX4" s="96"/>
-      <c r="AY4" s="94">
+      <c r="AS4" s="120"/>
+      <c r="AT4" s="120"/>
+      <c r="AU4" s="120"/>
+      <c r="AV4" s="120"/>
+      <c r="AW4" s="120"/>
+      <c r="AX4" s="121"/>
+      <c r="AY4" s="119">
         <f>AY5</f>
         <v>43612</v>
       </c>
-      <c r="AZ4" s="95"/>
-      <c r="BA4" s="95"/>
-      <c r="BB4" s="95"/>
-      <c r="BC4" s="95"/>
-      <c r="BD4" s="95"/>
-      <c r="BE4" s="96"/>
-      <c r="BF4" s="94">
+      <c r="AZ4" s="120"/>
+      <c r="BA4" s="120"/>
+      <c r="BB4" s="120"/>
+      <c r="BC4" s="120"/>
+      <c r="BD4" s="120"/>
+      <c r="BE4" s="121"/>
+      <c r="BF4" s="119">
         <f>BF5</f>
         <v>43619</v>
       </c>
-      <c r="BG4" s="95"/>
-      <c r="BH4" s="95"/>
-      <c r="BI4" s="95"/>
-      <c r="BJ4" s="95"/>
-      <c r="BK4" s="95"/>
-      <c r="BL4" s="96"/>
+      <c r="BG4" s="120"/>
+      <c r="BH4" s="120"/>
+      <c r="BI4" s="120"/>
+      <c r="BJ4" s="120"/>
+      <c r="BK4" s="120"/>
+      <c r="BL4" s="121"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
+      <c r="B5" s="125"/>
+      <c r="C5" s="125"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="125"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43570</v>
@@ -5908,6 +6069,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -5915,11 +6081,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D49">
     <cfRule type="dataBar" priority="14">
@@ -6095,10 +6256,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE1CF35-F31E-4918-8904-B18DF430CA8D}">
-  <dimension ref="A1:T53"/>
+  <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6107,10 +6268,11 @@
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="130"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="101" t="s">
+    <row r="1" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="91" t="s">
         <v>106</v>
       </c>
       <c r="B1" s="1"/>
@@ -6118,1078 +6280,1296 @@
       <c r="D1" s="4"/>
       <c r="E1" s="47"/>
     </row>
-    <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="97">
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="135">
         <v>43570</v>
       </c>
-      <c r="E3" s="97"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="103" t="s">
+      <c r="E2" s="136"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="134" t="s">
         <v>108</v>
       </c>
-      <c r="J3" s="104" t="s">
+      <c r="J2" s="131" t="s">
         <v>109</v>
       </c>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="98"/>
-      <c r="R3" s="98"/>
-      <c r="S3" s="98"/>
-      <c r="T3" s="98"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="83" t="s">
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="137"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="I3" s="134"/>
+      <c r="J3" s="131"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="137"/>
+      <c r="B4" s="137"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="89">
+        <v>43570</v>
+      </c>
+      <c r="G4" s="89">
+        <v>43577</v>
+      </c>
+      <c r="H4" s="89">
+        <v>43584</v>
+      </c>
+      <c r="I4" s="89">
+        <v>43591</v>
+      </c>
+      <c r="J4" s="132">
+        <v>43598</v>
+      </c>
+      <c r="K4" s="89">
+        <v>43605</v>
+      </c>
+      <c r="L4" s="89">
+        <v>43612</v>
+      </c>
+      <c r="M4" s="89">
+        <v>43619</v>
+      </c>
+      <c r="N4" s="89">
+        <v>43626</v>
+      </c>
+      <c r="O4" s="89">
+        <v>43633</v>
+      </c>
+      <c r="P4" s="89">
+        <v>43640</v>
+      </c>
+      <c r="Q4" s="89">
+        <v>43647</v>
+      </c>
+      <c r="R4" s="89">
+        <v>43654</v>
+      </c>
+      <c r="S4" s="89">
+        <v>43661</v>
+      </c>
+      <c r="T4" s="89">
+        <v>43668</v>
+      </c>
+      <c r="U4" s="129" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="7">
-        <v>1</v>
-      </c>
-      <c r="I4" s="103"/>
-      <c r="J4" s="104"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="90"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="99">
-        <v>43570</v>
-      </c>
-      <c r="G5" s="99">
-        <v>43577</v>
-      </c>
-      <c r="H5" s="99">
-        <v>43584</v>
-      </c>
-      <c r="I5" s="99">
-        <v>43591</v>
-      </c>
-      <c r="J5" s="99">
-        <v>43598</v>
-      </c>
-      <c r="K5" s="99">
-        <v>43605</v>
-      </c>
-      <c r="L5" s="99">
-        <v>43612</v>
-      </c>
-      <c r="M5" s="99">
-        <v>43619</v>
-      </c>
-      <c r="N5" s="99">
-        <v>43626</v>
-      </c>
-      <c r="O5" s="99">
-        <v>43633</v>
-      </c>
-      <c r="P5" s="99">
-        <v>43640</v>
-      </c>
-      <c r="Q5" s="99">
-        <v>43647</v>
-      </c>
-      <c r="R5" s="99">
-        <v>43654</v>
-      </c>
-      <c r="S5" s="99">
-        <v>43661</v>
-      </c>
-      <c r="T5" s="99">
-        <v>43668</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="C5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="90" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" s="90" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="90" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" s="133" t="s">
+        <v>95</v>
+      </c>
+      <c r="K5" s="90" t="s">
+        <v>96</v>
+      </c>
+      <c r="L5" s="90" t="s">
+        <v>97</v>
+      </c>
+      <c r="M5" s="90" t="s">
+        <v>98</v>
+      </c>
+      <c r="N5" s="90" t="s">
+        <v>99</v>
+      </c>
+      <c r="O5" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="P5" s="90" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q5" s="90" t="s">
+        <v>102</v>
+      </c>
+      <c r="R5" s="90" t="s">
+        <v>103</v>
+      </c>
+      <c r="S5" s="90" t="s">
+        <v>104</v>
+      </c>
+      <c r="T5" s="90" t="s">
+        <v>105</v>
+      </c>
+      <c r="U5" s="129"/>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="93" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="100" t="s">
-        <v>91</v>
-      </c>
-      <c r="G6" s="100" t="s">
-        <v>92</v>
-      </c>
-      <c r="H6" s="100" t="s">
-        <v>93</v>
-      </c>
-      <c r="I6" s="100" t="s">
-        <v>94</v>
-      </c>
-      <c r="J6" s="100" t="s">
-        <v>95</v>
-      </c>
-      <c r="K6" s="100" t="s">
-        <v>96</v>
-      </c>
-      <c r="L6" s="100" t="s">
-        <v>97</v>
-      </c>
-      <c r="M6" s="100" t="s">
-        <v>98</v>
-      </c>
-      <c r="N6" s="100" t="s">
-        <v>99</v>
-      </c>
-      <c r="O6" s="100" t="s">
-        <v>100</v>
-      </c>
-      <c r="P6" s="100" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q6" s="100" t="s">
-        <v>102</v>
-      </c>
-      <c r="R6" s="100" t="s">
-        <v>103</v>
-      </c>
-      <c r="S6" s="100" t="s">
-        <v>104</v>
-      </c>
-      <c r="T6" s="100" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="105" t="s">
+    </row>
+    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="94" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="106" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="107"/>
-      <c r="C8" s="108"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="110"/>
-      <c r="F8" s="108"/>
-      <c r="G8" s="108"/>
-      <c r="H8" s="108"/>
-      <c r="I8" s="108"/>
-      <c r="J8" s="108"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="111" t="s">
+      <c r="B7" s="95"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="96"/>
+      <c r="O7" s="96"/>
+      <c r="P7" s="96"/>
+      <c r="Q7" s="96"/>
+      <c r="R7" s="96"/>
+      <c r="S7" s="96"/>
+      <c r="T7" s="96"/>
+      <c r="U7" s="19"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="112" t="s">
+      <c r="B8" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="113">
+      <c r="C8" s="101">
         <v>0.5</v>
       </c>
-      <c r="D9" s="114">
+      <c r="D8" s="102">
         <f>Project_Start</f>
         <v>43570</v>
       </c>
-      <c r="E9" s="114">
-        <f>D9+12</f>
+      <c r="E8" s="138">
+        <f>D8+12</f>
         <v>43582</v>
       </c>
-      <c r="F9" s="115"/>
-      <c r="G9" s="115"/>
-      <c r="H9" s="115"/>
-      <c r="I9" s="116"/>
-      <c r="J9" s="117"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="111" t="s">
+      <c r="F8" s="139"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="140"/>
+      <c r="J8" s="158"/>
+      <c r="K8" s="157"/>
+      <c r="L8" s="140"/>
+      <c r="M8" s="140"/>
+      <c r="N8" s="140"/>
+      <c r="O8" s="140"/>
+      <c r="P8" s="140"/>
+      <c r="Q8" s="140"/>
+      <c r="R8" s="140"/>
+      <c r="S8" s="140"/>
+      <c r="T8" s="140"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="118" t="s">
+      <c r="B9" s="103" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="113">
-        <v>0.01</v>
-      </c>
-      <c r="D10" s="114">
+      <c r="C9" s="101">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="102">
         <v>43581</v>
       </c>
-      <c r="E10" s="114">
+      <c r="E9" s="138">
+        <f>D9+7</f>
+        <v>43588</v>
+      </c>
+      <c r="F9" s="140"/>
+      <c r="G9" s="141"/>
+      <c r="H9" s="141"/>
+      <c r="I9" s="140"/>
+      <c r="J9" s="158"/>
+      <c r="K9" s="157"/>
+      <c r="L9" s="140"/>
+      <c r="M9" s="140"/>
+      <c r="N9" s="140"/>
+      <c r="O9" s="140"/>
+      <c r="P9" s="140"/>
+      <c r="Q9" s="140"/>
+      <c r="R9" s="140"/>
+      <c r="S9" s="140"/>
+      <c r="T9" s="140"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="99" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="103" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="101">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="102">
+        <v>43581</v>
+      </c>
+      <c r="E10" s="138">
         <f>D10+7</f>
         <v>43588</v>
       </c>
-      <c r="F10" s="116"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="116"/>
-      <c r="J10" s="117"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="111" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="118" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="113">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="114">
-        <v>43581</v>
-      </c>
-      <c r="E11" s="114">
-        <f>D11+7</f>
-        <v>43588</v>
-      </c>
-      <c r="F11" s="119"/>
-      <c r="G11" s="116"/>
-      <c r="H11" s="116"/>
-      <c r="I11" s="116"/>
-      <c r="J11" s="117"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="111" t="s">
+      <c r="F10" s="141"/>
+      <c r="G10" s="140"/>
+      <c r="H10" s="140"/>
+      <c r="I10" s="140"/>
+      <c r="J10" s="158"/>
+      <c r="K10" s="157"/>
+      <c r="L10" s="140"/>
+      <c r="M10" s="140"/>
+      <c r="N10" s="140"/>
+      <c r="O10" s="140"/>
+      <c r="P10" s="140"/>
+      <c r="Q10" s="140"/>
+      <c r="R10" s="140"/>
+      <c r="S10" s="140"/>
+      <c r="T10" s="140"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="120" t="s">
-        <v>117</v>
-      </c>
-      <c r="C12" s="113"/>
-      <c r="D12" s="114">
+      <c r="B11" s="104" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="101">
+        <v>0</v>
+      </c>
+      <c r="D11" s="102">
         <v>43599</v>
       </c>
-      <c r="E12" s="114">
-        <f>D12+4</f>
+      <c r="E11" s="138">
+        <f>D11+4</f>
         <v>43603</v>
       </c>
-      <c r="F12" s="116"/>
-      <c r="G12" s="116"/>
-      <c r="H12" s="116"/>
-      <c r="I12" s="116"/>
-      <c r="J12" s="121" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="111" t="s">
+      <c r="F11" s="140"/>
+      <c r="G11" s="140"/>
+      <c r="H11" s="140"/>
+      <c r="I11" s="140"/>
+      <c r="J11" s="159" t="s">
+        <v>113</v>
+      </c>
+      <c r="K11" s="157"/>
+      <c r="L11" s="140"/>
+      <c r="M11" s="140"/>
+      <c r="N11" s="140"/>
+      <c r="O11" s="140"/>
+      <c r="P11" s="140"/>
+      <c r="Q11" s="140"/>
+      <c r="R11" s="140"/>
+      <c r="S11" s="140"/>
+      <c r="T11" s="140"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="122" t="s">
+      <c r="B12" s="105" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="113">
+      <c r="C12" s="101">
         <v>1</v>
       </c>
-      <c r="D13" s="114">
-        <f>D9</f>
+      <c r="D12" s="102">
+        <f>D8</f>
         <v>43570</v>
       </c>
-      <c r="E13" s="114">
+      <c r="E12" s="138">
+        <f>D12+12</f>
+        <v>43582</v>
+      </c>
+      <c r="F12" s="142"/>
+      <c r="G12" s="142"/>
+      <c r="H12" s="142"/>
+      <c r="I12" s="140"/>
+      <c r="J12" s="158"/>
+      <c r="K12" s="157"/>
+      <c r="L12" s="140"/>
+      <c r="M12" s="140"/>
+      <c r="N12" s="140"/>
+      <c r="O12" s="140"/>
+      <c r="P12" s="140"/>
+      <c r="Q12" s="140"/>
+      <c r="R12" s="140"/>
+      <c r="S12" s="140"/>
+      <c r="T12" s="140"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="99" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="105" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="101">
+        <v>1</v>
+      </c>
+      <c r="D13" s="102">
+        <v>43570</v>
+      </c>
+      <c r="E13" s="138">
         <f>D13+12</f>
         <v>43582</v>
       </c>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="116"/>
-      <c r="J13" s="117"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="111" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="122" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="113">
+      <c r="F13" s="140"/>
+      <c r="G13" s="142"/>
+      <c r="H13" s="142"/>
+      <c r="I13" s="142"/>
+      <c r="J13" s="158"/>
+      <c r="K13" s="157"/>
+      <c r="L13" s="140"/>
+      <c r="M13" s="140"/>
+      <c r="N13" s="140"/>
+      <c r="O13" s="140"/>
+      <c r="P13" s="140"/>
+      <c r="Q13" s="140"/>
+      <c r="R13" s="140"/>
+      <c r="S13" s="140"/>
+      <c r="T13" s="140"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="99" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="103" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="101">
         <v>1</v>
       </c>
-      <c r="D14" s="114">
+      <c r="D14" s="102">
         <v>43570</v>
       </c>
-      <c r="E14" s="114">
+      <c r="E14" s="138">
         <f>D14+12</f>
         <v>43582</v>
       </c>
-      <c r="F14" s="116"/>
-      <c r="G14" s="123"/>
-      <c r="H14" s="123"/>
-      <c r="I14" s="123"/>
-      <c r="J14" s="117"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="111" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="118" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="113">
+      <c r="F14" s="141"/>
+      <c r="G14" s="140"/>
+      <c r="H14" s="140"/>
+      <c r="I14" s="140"/>
+      <c r="J14" s="158"/>
+      <c r="K14" s="157"/>
+      <c r="L14" s="140"/>
+      <c r="M14" s="140"/>
+      <c r="N14" s="140"/>
+      <c r="O14" s="140"/>
+      <c r="P14" s="140"/>
+      <c r="Q14" s="140"/>
+      <c r="R14" s="140"/>
+      <c r="S14" s="140"/>
+      <c r="T14" s="140"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="99" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="105" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="101">
+        <v>0.1</v>
+      </c>
+      <c r="D15" s="102">
+        <f>D12</f>
+        <v>43570</v>
+      </c>
+      <c r="E15" s="138">
+        <f>D15+32</f>
+        <v>43602</v>
+      </c>
+      <c r="F15" s="142"/>
+      <c r="G15" s="142"/>
+      <c r="H15" s="142"/>
+      <c r="I15" s="142"/>
+      <c r="J15" s="160" t="s">
+        <v>113</v>
+      </c>
+      <c r="K15" s="157"/>
+      <c r="L15" s="140"/>
+      <c r="M15" s="140"/>
+      <c r="N15" s="140"/>
+      <c r="O15" s="140"/>
+      <c r="P15" s="140"/>
+      <c r="Q15" s="140"/>
+      <c r="R15" s="140"/>
+      <c r="S15" s="140"/>
+      <c r="T15" s="140"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="99" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="107" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="101">
+        <v>0</v>
+      </c>
+      <c r="D16" s="102">
+        <f>E14</f>
+        <v>43582</v>
+      </c>
+      <c r="E16" s="138">
+        <f>D16+12</f>
+        <v>43594</v>
+      </c>
+      <c r="F16" s="140"/>
+      <c r="G16" s="141"/>
+      <c r="H16" s="141"/>
+      <c r="I16" s="140"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="157"/>
+      <c r="L16" s="140"/>
+      <c r="M16" s="140"/>
+      <c r="N16" s="140"/>
+      <c r="O16" s="140"/>
+      <c r="P16" s="140"/>
+      <c r="Q16" s="140"/>
+      <c r="R16" s="140"/>
+      <c r="S16" s="140"/>
+      <c r="T16" s="140"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="99" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="108" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="101">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="102"/>
+      <c r="E17" s="138"/>
+      <c r="F17" s="143"/>
+      <c r="G17" s="143"/>
+      <c r="H17" s="143"/>
+      <c r="I17" s="140"/>
+      <c r="J17" s="158"/>
+      <c r="K17" s="157"/>
+      <c r="L17" s="140"/>
+      <c r="M17" s="140"/>
+      <c r="N17" s="140"/>
+      <c r="O17" s="140"/>
+      <c r="P17" s="140"/>
+      <c r="Q17" s="140"/>
+      <c r="R17" s="140"/>
+      <c r="S17" s="140"/>
+      <c r="T17" s="140"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="108" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="101">
         <v>1</v>
       </c>
-      <c r="D15" s="114">
-        <v>43570</v>
-      </c>
-      <c r="E15" s="114">
-        <f>D15+12</f>
-        <v>43582</v>
-      </c>
-      <c r="F15" s="119"/>
-      <c r="G15" s="116"/>
-      <c r="H15" s="116"/>
-      <c r="I15" s="116"/>
-      <c r="J15" s="117"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="111" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="122" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="113">
-        <v>0.1</v>
-      </c>
-      <c r="D16" s="114">
+      <c r="D18" s="102"/>
+      <c r="E18" s="138"/>
+      <c r="F18" s="140"/>
+      <c r="G18" s="140"/>
+      <c r="H18" s="143"/>
+      <c r="I18" s="143"/>
+      <c r="J18" s="158"/>
+      <c r="K18" s="157"/>
+      <c r="L18" s="140"/>
+      <c r="M18" s="140"/>
+      <c r="N18" s="140"/>
+      <c r="O18" s="140"/>
+      <c r="P18" s="140"/>
+      <c r="Q18" s="140"/>
+      <c r="R18" s="140"/>
+      <c r="S18" s="140"/>
+      <c r="T18" s="140"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="110" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="101">
+        <v>1</v>
+      </c>
+      <c r="D19" s="102">
         <f>D13</f>
         <v>43570</v>
       </c>
-      <c r="E16" s="114">
-        <f>D16+32</f>
-        <v>43602</v>
-      </c>
-      <c r="F16" s="123"/>
-      <c r="G16" s="123"/>
-      <c r="H16" s="123"/>
-      <c r="I16" s="123"/>
-      <c r="J16" s="124" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="111" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="125" t="s">
+      <c r="E19" s="138">
+        <f>D19+26</f>
+        <v>43596</v>
+      </c>
+      <c r="F19" s="144"/>
+      <c r="G19" s="144"/>
+      <c r="H19" s="144"/>
+      <c r="I19" s="144"/>
+      <c r="J19" s="159" t="s">
+        <v>113</v>
+      </c>
+      <c r="K19" s="157"/>
+      <c r="L19" s="140"/>
+      <c r="M19" s="140"/>
+      <c r="N19" s="140"/>
+      <c r="O19" s="140"/>
+      <c r="P19" s="140"/>
+      <c r="Q19" s="140"/>
+      <c r="R19" s="140"/>
+      <c r="S19" s="140"/>
+      <c r="T19" s="140"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="109" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="101">
+        <v>1</v>
+      </c>
+      <c r="D20" s="102">
+        <f>D19</f>
+        <v>43570</v>
+      </c>
+      <c r="E20" s="138">
+        <f>D20+12</f>
+        <v>43582</v>
+      </c>
+      <c r="F20" s="145"/>
+      <c r="G20" s="145"/>
+      <c r="H20" s="140"/>
+      <c r="I20" s="140"/>
+      <c r="J20" s="158"/>
+      <c r="K20" s="157"/>
+      <c r="L20" s="140"/>
+      <c r="M20" s="140"/>
+      <c r="N20" s="140"/>
+      <c r="O20" s="140"/>
+      <c r="P20" s="140"/>
+      <c r="Q20" s="140"/>
+      <c r="R20" s="140"/>
+      <c r="S20" s="140"/>
+      <c r="T20" s="140"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="99" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="110" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="113">
-        <v>0</v>
-      </c>
-      <c r="D17" s="114">
-        <f>E15</f>
-        <v>43582</v>
-      </c>
-      <c r="E17" s="114">
-        <f>D17+12</f>
-        <v>43594</v>
-      </c>
-      <c r="F17" s="116"/>
-      <c r="G17" s="119"/>
-      <c r="H17" s="119"/>
-      <c r="I17" s="116"/>
-      <c r="J17" s="117"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="111" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="126" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="113">
+      <c r="C21" s="101">
+        <v>1</v>
+      </c>
+      <c r="D21" s="102"/>
+      <c r="E21" s="138"/>
+      <c r="F21" s="144"/>
+      <c r="G21" s="140"/>
+      <c r="H21" s="140"/>
+      <c r="I21" s="140"/>
+      <c r="J21" s="158"/>
+      <c r="K21" s="157"/>
+      <c r="L21" s="140"/>
+      <c r="M21" s="140"/>
+      <c r="N21" s="140"/>
+      <c r="O21" s="140"/>
+      <c r="P21" s="140"/>
+      <c r="Q21" s="140"/>
+      <c r="R21" s="140"/>
+      <c r="S21" s="140"/>
+      <c r="T21" s="140"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="99" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="118" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="101">
         <v>0.5</v>
       </c>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="127"/>
-      <c r="G18" s="127"/>
-      <c r="H18" s="127"/>
-      <c r="I18" s="116"/>
-      <c r="J18" s="117"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="111" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="126" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="113"/>
-      <c r="D19" s="114"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="116"/>
-      <c r="G19" s="116"/>
-      <c r="H19" s="127"/>
-      <c r="I19" s="127"/>
-      <c r="J19" s="117"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="111" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="131" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="113">
-        <v>0.7</v>
-      </c>
-      <c r="D20" s="114">
-        <f>D14</f>
-        <v>43570</v>
-      </c>
-      <c r="E20" s="114">
-        <f>D20+26</f>
-        <v>43596</v>
-      </c>
-      <c r="F20" s="128"/>
-      <c r="G20" s="128"/>
-      <c r="H20" s="128"/>
-      <c r="I20" s="128"/>
-      <c r="J20" s="121" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="111" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="129" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="113">
-        <v>1</v>
-      </c>
-      <c r="D21" s="114">
+      <c r="D22" s="102">
         <f>D20</f>
         <v>43570</v>
       </c>
-      <c r="E21" s="114">
-        <f>D21+12</f>
+      <c r="E22" s="138">
+        <f>D22+12</f>
         <v>43582</v>
       </c>
-      <c r="F21" s="130"/>
-      <c r="G21" s="130"/>
-      <c r="H21" s="116"/>
-      <c r="I21" s="116"/>
-      <c r="J21" s="117"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="111" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="131" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="113">
-        <v>1</v>
-      </c>
-      <c r="D22" s="114"/>
-      <c r="E22" s="114"/>
-      <c r="F22" s="128"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="116"/>
-      <c r="I22" s="116"/>
-      <c r="J22" s="117"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="146"/>
+      <c r="H22" s="146"/>
+      <c r="I22" s="140"/>
+      <c r="J22" s="158"/>
+      <c r="K22" s="157"/>
+      <c r="L22" s="140"/>
+      <c r="M22" s="140"/>
+      <c r="N22" s="140"/>
+      <c r="O22" s="140"/>
+      <c r="P22" s="140"/>
+      <c r="Q22" s="140"/>
+      <c r="R22" s="140"/>
+      <c r="S22" s="140"/>
+      <c r="T22" s="140"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="111" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="140" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="113">
-        <v>0.5</v>
-      </c>
-      <c r="D23" s="114">
-        <f>D21</f>
-        <v>43570</v>
-      </c>
-      <c r="E23" s="114">
-        <f>D23+12</f>
-        <v>43582</v>
+      <c r="A23" s="99" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="110" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="101">
+        <v>0</v>
+      </c>
+      <c r="D23" s="102">
+        <v>43597</v>
+      </c>
+      <c r="E23" s="138">
+        <f>D23+4</f>
+        <v>43601</v>
       </c>
       <c r="F23" s="140"/>
       <c r="G23" s="140"/>
       <c r="H23" s="140"/>
-      <c r="I23" s="116"/>
-      <c r="J23" s="117"/>
+      <c r="I23" s="144"/>
+      <c r="J23" s="159" t="s">
+        <v>113</v>
+      </c>
+      <c r="K23" s="157"/>
+      <c r="L23" s="140"/>
+      <c r="M23" s="140"/>
+      <c r="N23" s="140"/>
+      <c r="O23" s="140"/>
+      <c r="P23" s="140"/>
+      <c r="Q23" s="140"/>
+      <c r="R23" s="140"/>
+      <c r="S23" s="140"/>
+      <c r="T23" s="140"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="111" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="131" t="s">
+      <c r="A24" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="113">
-        <v>0</v>
-      </c>
-      <c r="D24" s="114">
-        <v>43597</v>
-      </c>
-      <c r="E24" s="114">
-        <f>D24+4</f>
-        <v>43601</v>
-      </c>
-      <c r="F24" s="116"/>
-      <c r="G24" s="116"/>
-      <c r="H24" s="116"/>
-      <c r="I24" s="128"/>
-      <c r="J24" s="121" t="s">
-        <v>114</v>
-      </c>
+      <c r="B24" s="109" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="101">
+        <v>1</v>
+      </c>
+      <c r="D24" s="102">
+        <v>43590</v>
+      </c>
+      <c r="E24" s="138">
+        <f>D24</f>
+        <v>43590</v>
+      </c>
+      <c r="F24" s="147"/>
+      <c r="G24" s="147"/>
+      <c r="H24" s="148" t="s">
+        <v>113</v>
+      </c>
+      <c r="I24" s="140"/>
+      <c r="J24" s="158"/>
+      <c r="K24" s="157"/>
+      <c r="L24" s="140"/>
+      <c r="M24" s="140"/>
+      <c r="N24" s="140"/>
+      <c r="O24" s="140"/>
+      <c r="P24" s="140"/>
+      <c r="Q24" s="140"/>
+      <c r="R24" s="140"/>
+      <c r="S24" s="140"/>
+      <c r="T24" s="140"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="111" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="109" t="s">
         <v>118</v>
       </c>
-      <c r="B25" s="129" t="s">
-        <v>119</v>
-      </c>
-      <c r="C25" s="113">
-        <v>1</v>
-      </c>
-      <c r="D25" s="114">
-        <v>43590</v>
-      </c>
-      <c r="E25" s="114">
+      <c r="C25" s="101"/>
+      <c r="D25" s="102">
+        <v>43604</v>
+      </c>
+      <c r="E25" s="138">
         <f>D25</f>
-        <v>43590</v>
-      </c>
-      <c r="F25" s="129"/>
-      <c r="G25" s="129"/>
-      <c r="H25" s="132" t="s">
-        <v>114</v>
-      </c>
-      <c r="I25" s="116"/>
-      <c r="J25" s="117"/>
+        <v>43604</v>
+      </c>
+      <c r="F25" s="140"/>
+      <c r="G25" s="140"/>
+      <c r="H25" s="140"/>
+      <c r="I25" s="147"/>
+      <c r="J25" s="161" t="s">
+        <v>113</v>
+      </c>
+      <c r="K25" s="157"/>
+      <c r="L25" s="140"/>
+      <c r="M25" s="140"/>
+      <c r="N25" s="140"/>
+      <c r="O25" s="140"/>
+      <c r="P25" s="140"/>
+      <c r="Q25" s="140"/>
+      <c r="R25" s="140"/>
+      <c r="S25" s="140"/>
+      <c r="T25" s="140"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="133" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" s="129" t="s">
-        <v>119</v>
-      </c>
-      <c r="C26" s="113"/>
-      <c r="D26" s="114">
+      <c r="A26" s="111" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="110" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="101"/>
+      <c r="D26" s="102">
         <v>43604</v>
       </c>
-      <c r="E26" s="114">
+      <c r="E26" s="138">
         <f>D26</f>
         <v>43604</v>
       </c>
-      <c r="F26" s="116"/>
-      <c r="G26" s="116"/>
-      <c r="H26" s="116"/>
-      <c r="I26" s="129"/>
-      <c r="J26" s="132" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="133" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="131" t="s">
-        <v>117</v>
-      </c>
-      <c r="C27" s="113"/>
-      <c r="D27" s="114">
-        <v>43604</v>
-      </c>
-      <c r="E27" s="114">
-        <f>D27</f>
-        <v>43604</v>
-      </c>
-      <c r="F27" s="116"/>
-      <c r="G27" s="116"/>
-      <c r="H27" s="116"/>
-      <c r="I27" s="128"/>
-      <c r="J27" s="121" t="s">
-        <v>114</v>
-      </c>
+      <c r="F26" s="140"/>
+      <c r="G26" s="140"/>
+      <c r="H26" s="140"/>
+      <c r="I26" s="144"/>
+      <c r="J26" s="159" t="s">
+        <v>113</v>
+      </c>
+      <c r="K26" s="157"/>
+      <c r="L26" s="140"/>
+      <c r="M26" s="140"/>
+      <c r="N26" s="140"/>
+      <c r="O26" s="140"/>
+      <c r="P26" s="140"/>
+      <c r="Q26" s="140"/>
+      <c r="R26" s="140"/>
+      <c r="S26" s="140"/>
+      <c r="T26" s="140"/>
+    </row>
+    <row r="27" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="113"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="115"/>
+      <c r="E27" s="116"/>
+      <c r="F27" s="149"/>
+      <c r="G27" s="149"/>
+      <c r="H27" s="149"/>
+      <c r="I27" s="149"/>
+      <c r="J27" s="149"/>
+      <c r="K27" s="149"/>
+      <c r="L27" s="149"/>
+      <c r="M27" s="149"/>
+      <c r="N27" s="149"/>
+      <c r="O27" s="149"/>
+      <c r="P27" s="149"/>
+      <c r="Q27" s="149"/>
+      <c r="R27" s="149"/>
+      <c r="S27" s="149"/>
+      <c r="T27" s="149"/>
     </row>
     <row r="28" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="134" t="s">
-        <v>120</v>
-      </c>
-      <c r="B28" s="135"/>
-      <c r="C28" s="136"/>
-      <c r="D28" s="137"/>
-      <c r="E28" s="138"/>
-      <c r="F28" s="136"/>
-      <c r="G28" s="136"/>
-      <c r="H28" s="136"/>
-      <c r="I28" s="136"/>
-      <c r="J28" s="136"/>
-      <c r="K28" s="136"/>
-      <c r="L28" s="136"/>
-      <c r="M28" s="136"/>
-      <c r="N28" s="136"/>
-      <c r="O28" s="136"/>
-      <c r="P28" s="136"/>
-      <c r="Q28" s="136"/>
-      <c r="R28" s="136"/>
-      <c r="S28" s="136"/>
-      <c r="T28" s="136"/>
+      <c r="A28" s="86" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="106" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="27">
+        <v>0</v>
+      </c>
+      <c r="D28" s="66">
+        <f>D26+1</f>
+        <v>43605</v>
+      </c>
+      <c r="E28" s="66">
+        <f>D28+4</f>
+        <v>43609</v>
+      </c>
+      <c r="F28" s="142"/>
+      <c r="G28" s="142"/>
+      <c r="H28" s="142"/>
+      <c r="I28" s="140"/>
+      <c r="J28" s="158"/>
+      <c r="K28" s="157"/>
+      <c r="L28" s="140"/>
+      <c r="M28" s="140"/>
+      <c r="N28" s="140"/>
+      <c r="O28" s="140"/>
+      <c r="P28" s="140"/>
+      <c r="Q28" s="140"/>
+      <c r="R28" s="140"/>
+      <c r="S28" s="140"/>
+      <c r="T28" s="140"/>
     </row>
     <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="86" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" s="73" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="106" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="27">
         <v>0</v>
       </c>
       <c r="D29" s="66">
-        <f>D27+1</f>
-        <v>43605</v>
+        <f>D28+2</f>
+        <v>43607</v>
       </c>
       <c r="E29" s="66">
-        <f>D29+4</f>
-        <v>43609</v>
-      </c>
-      <c r="F29" s="116"/>
-      <c r="G29" s="116"/>
-      <c r="H29" s="116"/>
-      <c r="I29" s="116"/>
-      <c r="J29" s="117"/>
-      <c r="K29" s="116"/>
-      <c r="L29" s="116"/>
-      <c r="M29" s="116"/>
-      <c r="N29" s="116"/>
-      <c r="O29" s="116"/>
-      <c r="P29" s="116"/>
-      <c r="Q29" s="116"/>
-      <c r="R29" s="116"/>
-      <c r="S29" s="116"/>
-      <c r="T29" s="116"/>
+        <f>D29+5</f>
+        <v>43612</v>
+      </c>
+      <c r="F29" s="142"/>
+      <c r="G29" s="142"/>
+      <c r="H29" s="142"/>
+      <c r="I29" s="140"/>
+      <c r="J29" s="158"/>
+      <c r="K29" s="157"/>
+      <c r="L29" s="140"/>
+      <c r="M29" s="140"/>
+      <c r="N29" s="140"/>
+      <c r="O29" s="140"/>
+      <c r="P29" s="140"/>
+      <c r="Q29" s="140"/>
+      <c r="R29" s="140"/>
+      <c r="S29" s="140"/>
+      <c r="T29" s="140"/>
     </row>
     <row r="30" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="86" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="27">
-        <v>0</v>
-      </c>
+      <c r="C30" s="27"/>
       <c r="D30" s="66">
-        <f>D29+2</f>
-        <v>43607</v>
+        <f>E29</f>
+        <v>43612</v>
       </c>
       <c r="E30" s="66">
-        <f>D30+5</f>
-        <v>43612</v>
-      </c>
-      <c r="F30" s="116"/>
-      <c r="G30" s="116"/>
-      <c r="H30" s="116"/>
-      <c r="I30" s="116"/>
-      <c r="J30" s="117"/>
-      <c r="K30" s="116"/>
-      <c r="L30" s="116"/>
-      <c r="M30" s="116"/>
-      <c r="N30" s="116"/>
-      <c r="O30" s="116"/>
-      <c r="P30" s="116"/>
-      <c r="Q30" s="116"/>
-      <c r="R30" s="116"/>
-      <c r="S30" s="116"/>
-      <c r="T30" s="116"/>
+        <f>D30+3</f>
+        <v>43615</v>
+      </c>
+      <c r="F30" s="140"/>
+      <c r="G30" s="142"/>
+      <c r="H30" s="142"/>
+      <c r="I30" s="142"/>
+      <c r="J30" s="158"/>
+      <c r="K30" s="157"/>
+      <c r="L30" s="140"/>
+      <c r="M30" s="140"/>
+      <c r="N30" s="140"/>
+      <c r="O30" s="140"/>
+      <c r="P30" s="140"/>
+      <c r="Q30" s="140"/>
+      <c r="R30" s="140"/>
+      <c r="S30" s="140"/>
+      <c r="T30" s="140"/>
     </row>
     <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="86" t="s">
         <v>121</v>
       </c>
-      <c r="B31" s="73" t="s">
-        <v>53</v>
+      <c r="B31" s="110" t="s">
+        <v>116</v>
       </c>
       <c r="C31" s="27"/>
-      <c r="D31" s="66">
-        <f>E30</f>
-        <v>43612</v>
-      </c>
-      <c r="E31" s="66">
-        <f>D31+3</f>
-        <v>43615</v>
-      </c>
-      <c r="F31" s="116"/>
-      <c r="G31" s="116"/>
-      <c r="H31" s="116"/>
-      <c r="I31" s="116"/>
-      <c r="J31" s="117"/>
-      <c r="K31" s="116"/>
-      <c r="L31" s="116"/>
-      <c r="M31" s="116"/>
-      <c r="N31" s="116"/>
-      <c r="O31" s="116"/>
-      <c r="P31" s="116"/>
-      <c r="Q31" s="116"/>
-      <c r="R31" s="116"/>
-      <c r="S31" s="116"/>
-      <c r="T31" s="116"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="140"/>
+      <c r="G31" s="140"/>
+      <c r="H31" s="140"/>
+      <c r="I31" s="150"/>
+      <c r="J31" s="159" t="s">
+        <v>113</v>
+      </c>
+      <c r="K31" s="157"/>
+      <c r="L31" s="140"/>
+      <c r="M31" s="140"/>
+      <c r="N31" s="140"/>
+      <c r="O31" s="140"/>
+      <c r="P31" s="140"/>
+      <c r="Q31" s="140"/>
+      <c r="R31" s="140"/>
+      <c r="S31" s="140"/>
+      <c r="T31" s="140"/>
     </row>
     <row r="32" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="86" t="s">
-        <v>122</v>
-      </c>
-      <c r="B32" s="73" t="s">
-        <v>57</v>
+        <v>140</v>
+      </c>
+      <c r="B32" s="106" t="s">
+        <v>53</v>
       </c>
       <c r="C32" s="27"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="66"/>
-      <c r="F32" s="116"/>
-      <c r="G32" s="116"/>
-      <c r="H32" s="116"/>
-      <c r="I32" s="116"/>
-      <c r="J32" s="117"/>
-      <c r="K32" s="116"/>
-      <c r="L32" s="116"/>
-      <c r="M32" s="116"/>
-      <c r="N32" s="116"/>
-      <c r="O32" s="116"/>
-      <c r="P32" s="116"/>
-      <c r="Q32" s="116"/>
-      <c r="R32" s="116"/>
-      <c r="S32" s="116"/>
-      <c r="T32" s="116"/>
+      <c r="D32" s="66">
+        <f>D30</f>
+        <v>43612</v>
+      </c>
+      <c r="E32" s="66">
+        <f>D32+2</f>
+        <v>43614</v>
+      </c>
+      <c r="F32" s="140"/>
+      <c r="G32" s="140"/>
+      <c r="H32" s="140"/>
+      <c r="I32" s="140"/>
+      <c r="J32" s="158"/>
+      <c r="K32" s="157"/>
+      <c r="L32" s="140"/>
+      <c r="M32" s="140"/>
+      <c r="N32" s="140"/>
+      <c r="O32" s="140"/>
+      <c r="P32" s="140"/>
+      <c r="Q32" s="140"/>
+      <c r="R32" s="140"/>
+      <c r="S32" s="140"/>
+      <c r="T32" s="140"/>
     </row>
     <row r="33" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="86" t="s">
-        <v>123</v>
-      </c>
-      <c r="B33" s="73" t="s">
-        <v>53</v>
+        <v>122</v>
+      </c>
+      <c r="B33" s="110" t="s">
+        <v>116</v>
       </c>
       <c r="C33" s="27"/>
       <c r="D33" s="66">
-        <f>D31</f>
-        <v>43612</v>
+        <f>E32</f>
+        <v>43614</v>
       </c>
       <c r="E33" s="66">
-        <f>D33+2</f>
-        <v>43614</v>
-      </c>
-      <c r="F33" s="116"/>
-      <c r="G33" s="116"/>
-      <c r="H33" s="116"/>
-      <c r="I33" s="116"/>
-      <c r="J33" s="117"/>
-      <c r="K33" s="116"/>
-      <c r="L33" s="116"/>
-      <c r="M33" s="116"/>
-      <c r="N33" s="116"/>
-      <c r="O33" s="116"/>
-      <c r="P33" s="116"/>
-      <c r="Q33" s="116"/>
-      <c r="R33" s="116"/>
-      <c r="S33" s="116"/>
-      <c r="T33" s="116"/>
+        <f>D33+4</f>
+        <v>43618</v>
+      </c>
+      <c r="F33" s="140"/>
+      <c r="G33" s="140"/>
+      <c r="H33" s="140"/>
+      <c r="I33" s="150"/>
+      <c r="J33" s="166"/>
+      <c r="K33" s="162"/>
+      <c r="L33" s="150"/>
+      <c r="M33" s="140"/>
+      <c r="N33" s="140"/>
+      <c r="O33" s="140"/>
+      <c r="P33" s="140"/>
+      <c r="Q33" s="140"/>
+      <c r="R33" s="140"/>
+      <c r="S33" s="140"/>
+      <c r="T33" s="140"/>
     </row>
     <row r="34" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="86" t="s">
-        <v>124</v>
-      </c>
-      <c r="B34" s="73" t="s">
-        <v>57</v>
+        <v>141</v>
+      </c>
+      <c r="B34" s="118" t="s">
+        <v>73</v>
       </c>
       <c r="C34" s="27"/>
-      <c r="D34" s="66">
-        <f>E33</f>
-        <v>43614</v>
-      </c>
-      <c r="E34" s="66">
-        <f>D34+4</f>
-        <v>43618</v>
-      </c>
-      <c r="F34" s="116"/>
-      <c r="G34" s="116"/>
-      <c r="H34" s="116"/>
-      <c r="I34" s="116"/>
-      <c r="J34" s="117"/>
-      <c r="K34" s="116"/>
-      <c r="L34" s="116"/>
-      <c r="M34" s="116"/>
-      <c r="N34" s="116"/>
-      <c r="O34" s="116"/>
-      <c r="P34" s="116"/>
-      <c r="Q34" s="116"/>
-      <c r="R34" s="116"/>
-      <c r="S34" s="116"/>
-      <c r="T34" s="116"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="140"/>
+      <c r="G34" s="146"/>
+      <c r="H34" s="146"/>
+      <c r="I34" s="146"/>
+      <c r="J34" s="167"/>
+      <c r="K34" s="163"/>
+      <c r="L34" s="140"/>
+      <c r="M34" s="140"/>
+      <c r="N34" s="140"/>
+      <c r="O34" s="140"/>
+      <c r="P34" s="140"/>
+      <c r="Q34" s="140"/>
+      <c r="R34" s="140"/>
+      <c r="S34" s="140"/>
+      <c r="T34" s="140"/>
     </row>
     <row r="35" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="86" t="s">
-        <v>125</v>
-      </c>
-      <c r="B35" s="73" t="s">
-        <v>73</v>
+        <v>80</v>
+      </c>
+      <c r="B35" s="108" t="s">
+        <v>64</v>
       </c>
       <c r="C35" s="27"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="66"/>
-      <c r="F35" s="116"/>
-      <c r="G35" s="116"/>
-      <c r="H35" s="116"/>
-      <c r="I35" s="116"/>
-      <c r="J35" s="117"/>
-      <c r="K35" s="116"/>
-      <c r="L35" s="116"/>
-      <c r="M35" s="116"/>
-      <c r="N35" s="116"/>
-      <c r="O35" s="116"/>
-      <c r="P35" s="116"/>
-      <c r="Q35" s="116"/>
-      <c r="R35" s="116"/>
-      <c r="S35" s="116"/>
-      <c r="T35" s="116"/>
+      <c r="D35" s="66">
+        <f>D33</f>
+        <v>43614</v>
+      </c>
+      <c r="E35" s="66">
+        <f>E33</f>
+        <v>43618</v>
+      </c>
+      <c r="F35" s="140"/>
+      <c r="G35" s="140"/>
+      <c r="H35" s="143"/>
+      <c r="I35" s="143"/>
+      <c r="J35" s="168"/>
+      <c r="K35" s="164"/>
+      <c r="L35" s="143"/>
+      <c r="M35" s="140"/>
+      <c r="N35" s="140"/>
+      <c r="O35" s="140"/>
+      <c r="P35" s="140"/>
+      <c r="Q35" s="140"/>
+      <c r="R35" s="140"/>
+      <c r="S35" s="140"/>
+      <c r="T35" s="140"/>
     </row>
     <row r="36" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="86" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="73" t="s">
-        <v>64</v>
+        <v>123</v>
+      </c>
+      <c r="B36" s="107" t="s">
+        <v>52</v>
       </c>
       <c r="C36" s="27"/>
-      <c r="D36" s="66">
-        <f>D34</f>
-        <v>43614</v>
-      </c>
-      <c r="E36" s="66">
-        <f>E34</f>
-        <v>43618</v>
-      </c>
-      <c r="F36" s="116"/>
-      <c r="G36" s="116"/>
-      <c r="H36" s="116"/>
-      <c r="I36" s="116"/>
-      <c r="J36" s="117"/>
-      <c r="K36" s="116"/>
-      <c r="L36" s="116"/>
-      <c r="M36" s="116"/>
-      <c r="N36" s="116"/>
-      <c r="O36" s="116"/>
-      <c r="P36" s="116"/>
-      <c r="Q36" s="116"/>
-      <c r="R36" s="116"/>
-      <c r="S36" s="116"/>
-      <c r="T36" s="116"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="140"/>
+      <c r="G36" s="151"/>
+      <c r="H36" s="151"/>
+      <c r="I36" s="151"/>
+      <c r="J36" s="169"/>
+      <c r="K36" s="157"/>
+      <c r="L36" s="140"/>
+      <c r="M36" s="140"/>
+      <c r="N36" s="140"/>
+      <c r="O36" s="140"/>
+      <c r="P36" s="140"/>
+      <c r="Q36" s="140"/>
+      <c r="R36" s="140"/>
+      <c r="S36" s="140"/>
+      <c r="T36" s="140"/>
     </row>
     <row r="37" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="86" t="s">
-        <v>126</v>
-      </c>
-      <c r="B37" s="73" t="s">
-        <v>52</v>
+        <v>81</v>
+      </c>
+      <c r="B37" s="118" t="s">
+        <v>73</v>
       </c>
       <c r="C37" s="27"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="116"/>
-      <c r="G37" s="116"/>
-      <c r="H37" s="116"/>
-      <c r="I37" s="116"/>
-      <c r="J37" s="117"/>
-      <c r="K37" s="116"/>
-      <c r="L37" s="116"/>
-      <c r="M37" s="116"/>
-      <c r="N37" s="116"/>
-      <c r="O37" s="116"/>
-      <c r="P37" s="116"/>
-      <c r="Q37" s="116"/>
-      <c r="R37" s="116"/>
-      <c r="S37" s="116"/>
-      <c r="T37" s="116"/>
+      <c r="D37" s="66">
+        <f>D32</f>
+        <v>43612</v>
+      </c>
+      <c r="E37" s="66">
+        <f>D37+3</f>
+        <v>43615</v>
+      </c>
+      <c r="F37" s="140"/>
+      <c r="G37" s="140"/>
+      <c r="H37" s="140"/>
+      <c r="I37" s="146"/>
+      <c r="J37" s="167"/>
+      <c r="K37" s="165"/>
+      <c r="L37" s="146"/>
+      <c r="M37" s="140"/>
+      <c r="N37" s="140"/>
+      <c r="O37" s="140"/>
+      <c r="P37" s="140"/>
+      <c r="Q37" s="140"/>
+      <c r="R37" s="140"/>
+      <c r="S37" s="140"/>
+      <c r="T37" s="140"/>
     </row>
     <row r="38" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="86" t="s">
-        <v>81</v>
-      </c>
-      <c r="B38" s="73" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="66">
-        <f>D33</f>
-        <v>43612</v>
-      </c>
-      <c r="E38" s="66">
-        <f>D38+3</f>
+      <c r="A38" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" s="74"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="152"/>
+      <c r="G38" s="152"/>
+      <c r="H38" s="152"/>
+      <c r="I38" s="152"/>
+      <c r="J38" s="152"/>
+      <c r="K38" s="152"/>
+      <c r="L38" s="152"/>
+      <c r="M38" s="152"/>
+      <c r="N38" s="152"/>
+      <c r="O38" s="152"/>
+      <c r="P38" s="152"/>
+      <c r="Q38" s="152"/>
+      <c r="R38" s="152"/>
+      <c r="S38" s="152"/>
+      <c r="T38" s="152"/>
+    </row>
+    <row r="39" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="87" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="75" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="32"/>
+      <c r="D39" s="67">
+        <f>E37</f>
         <v>43615</v>
       </c>
-      <c r="F38" s="116"/>
-      <c r="G38" s="116"/>
-      <c r="H38" s="116"/>
-      <c r="I38" s="116"/>
-      <c r="J38" s="117"/>
-      <c r="K38" s="116"/>
-      <c r="L38" s="116"/>
-      <c r="M38" s="116"/>
-      <c r="N38" s="116"/>
-      <c r="O38" s="116"/>
-      <c r="P38" s="116"/>
-      <c r="Q38" s="116"/>
-      <c r="R38" s="116"/>
-      <c r="S38" s="116"/>
-      <c r="T38" s="116"/>
-    </row>
-    <row r="39" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="B39" s="74"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="29"/>
-      <c r="L39" s="29"/>
-      <c r="M39" s="29"/>
-      <c r="N39" s="29"/>
-      <c r="O39" s="29"/>
-      <c r="P39" s="29"/>
-      <c r="Q39" s="29"/>
-      <c r="R39" s="29"/>
-      <c r="S39" s="29"/>
-      <c r="T39" s="29"/>
+      <c r="E39" s="67">
+        <f>D39+5</f>
+        <v>43620</v>
+      </c>
+      <c r="F39" s="140"/>
+      <c r="G39" s="140"/>
+      <c r="H39" s="140"/>
+      <c r="I39" s="140"/>
+      <c r="J39" s="158"/>
+      <c r="K39" s="170"/>
+      <c r="L39" s="153"/>
+      <c r="M39" s="153"/>
+      <c r="N39" s="153"/>
+      <c r="O39" s="153"/>
+      <c r="P39" s="140"/>
+      <c r="Q39" s="140"/>
+      <c r="R39" s="140"/>
+      <c r="S39" s="140"/>
+      <c r="T39" s="140"/>
     </row>
     <row r="40" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="87" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B40" s="75" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C40" s="32"/>
-      <c r="D40" s="67">
-        <f>E38</f>
-        <v>43615</v>
-      </c>
-      <c r="E40" s="67">
-        <f>D40+5</f>
-        <v>43620</v>
-      </c>
-      <c r="F40" s="116"/>
-      <c r="G40" s="116"/>
-      <c r="H40" s="116"/>
-      <c r="I40" s="116"/>
-      <c r="J40" s="117"/>
-      <c r="K40" s="116"/>
-      <c r="L40" s="116"/>
-      <c r="M40" s="116"/>
-      <c r="N40" s="116"/>
-      <c r="O40" s="116"/>
-      <c r="P40" s="116"/>
-      <c r="Q40" s="116"/>
-      <c r="R40" s="116"/>
-      <c r="S40" s="116"/>
-      <c r="T40" s="116"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="140"/>
+      <c r="G40" s="140"/>
+      <c r="H40" s="140"/>
+      <c r="I40" s="140"/>
+      <c r="J40" s="158"/>
+      <c r="K40" s="157"/>
+      <c r="L40" s="140"/>
+      <c r="M40" s="153"/>
+      <c r="N40" s="153"/>
+      <c r="O40" s="153"/>
+      <c r="P40" s="153"/>
+      <c r="Q40" s="153"/>
+      <c r="R40" s="153"/>
+      <c r="S40" s="153"/>
+      <c r="T40" s="140"/>
     </row>
     <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="87" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="B41" s="75" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C41" s="32"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="67"/>
-      <c r="F41" s="116"/>
-      <c r="G41" s="116"/>
-      <c r="H41" s="116"/>
-      <c r="I41" s="116"/>
-      <c r="J41" s="117"/>
-      <c r="K41" s="116"/>
-      <c r="L41" s="116"/>
-      <c r="M41" s="116"/>
-      <c r="N41" s="116"/>
-      <c r="O41" s="116"/>
-      <c r="P41" s="116"/>
-      <c r="Q41" s="116"/>
-      <c r="R41" s="116"/>
-      <c r="S41" s="116"/>
-      <c r="T41" s="116"/>
+      <c r="D41" s="67">
+        <f>E39+1</f>
+        <v>43621</v>
+      </c>
+      <c r="E41" s="67">
+        <f>D41+4</f>
+        <v>43625</v>
+      </c>
+      <c r="F41" s="140"/>
+      <c r="G41" s="140"/>
+      <c r="H41" s="140"/>
+      <c r="I41" s="140"/>
+      <c r="J41" s="158"/>
+      <c r="K41" s="170"/>
+      <c r="L41" s="153"/>
+      <c r="M41" s="153"/>
+      <c r="N41" s="153"/>
+      <c r="O41" s="153"/>
+      <c r="P41" s="153"/>
+      <c r="Q41" s="153"/>
+      <c r="R41" s="153"/>
+      <c r="S41" s="153"/>
+      <c r="T41" s="153"/>
     </row>
     <row r="42" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="87" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B42" s="75" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C42" s="32"/>
-      <c r="D42" s="67">
-        <f>E40+1</f>
-        <v>43621</v>
-      </c>
-      <c r="E42" s="67">
-        <f>D42+4</f>
-        <v>43625</v>
-      </c>
-      <c r="F42" s="116"/>
-      <c r="G42" s="116"/>
-      <c r="H42" s="116"/>
-      <c r="I42" s="116"/>
-      <c r="J42" s="117"/>
-      <c r="K42" s="116"/>
-      <c r="L42" s="116"/>
-      <c r="M42" s="116"/>
-      <c r="N42" s="116"/>
-      <c r="O42" s="116"/>
-      <c r="P42" s="116"/>
-      <c r="Q42" s="116"/>
-      <c r="R42" s="116"/>
-      <c r="S42" s="116"/>
-      <c r="T42" s="116"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="140"/>
+      <c r="G42" s="140"/>
+      <c r="H42" s="140"/>
+      <c r="I42" s="140"/>
+      <c r="J42" s="158"/>
+      <c r="K42" s="170"/>
+      <c r="L42" s="153"/>
+      <c r="M42" s="153"/>
+      <c r="N42" s="153"/>
+      <c r="O42" s="153"/>
+      <c r="P42" s="153"/>
+      <c r="Q42" s="153"/>
+      <c r="R42" s="153"/>
+      <c r="S42" s="153"/>
+      <c r="T42" s="153"/>
     </row>
     <row r="43" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="87" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B43" s="75" t="s">
         <v>130</v>
@@ -7197,172 +7577,176 @@
       <c r="C43" s="32"/>
       <c r="D43" s="67"/>
       <c r="E43" s="67"/>
-      <c r="F43" s="116"/>
-      <c r="G43" s="116"/>
-      <c r="H43" s="116"/>
-      <c r="I43" s="116"/>
-      <c r="J43" s="117"/>
-      <c r="K43" s="116"/>
-      <c r="L43" s="116"/>
-      <c r="M43" s="116"/>
-      <c r="N43" s="116"/>
-      <c r="O43" s="116"/>
-      <c r="P43" s="116"/>
-      <c r="Q43" s="116"/>
-      <c r="R43" s="116"/>
-      <c r="S43" s="116"/>
-      <c r="T43" s="116"/>
+      <c r="F43" s="140"/>
+      <c r="G43" s="140"/>
+      <c r="H43" s="140"/>
+      <c r="I43" s="140"/>
+      <c r="J43" s="158"/>
+      <c r="K43" s="170"/>
+      <c r="L43" s="153"/>
+      <c r="M43" s="153"/>
+      <c r="N43" s="153"/>
+      <c r="O43" s="153"/>
+      <c r="P43" s="153"/>
+      <c r="Q43" s="140"/>
+      <c r="R43" s="140"/>
+      <c r="S43" s="140"/>
+      <c r="T43" s="140"/>
     </row>
     <row r="44" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="87" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="B44" s="75" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C44" s="32"/>
-      <c r="D44" s="67"/>
-      <c r="E44" s="67"/>
-      <c r="F44" s="116"/>
-      <c r="G44" s="116"/>
-      <c r="H44" s="116"/>
-      <c r="I44" s="116"/>
-      <c r="J44" s="117"/>
-      <c r="K44" s="116"/>
-      <c r="L44" s="116"/>
-      <c r="M44" s="116"/>
-      <c r="N44" s="116"/>
-      <c r="O44" s="116"/>
-      <c r="P44" s="116"/>
-      <c r="Q44" s="116"/>
-      <c r="R44" s="116"/>
-      <c r="S44" s="116"/>
-      <c r="T44" s="116"/>
+      <c r="D44" s="67">
+        <f>D41+5</f>
+        <v>43626</v>
+      </c>
+      <c r="E44" s="67">
+        <f>D44+5</f>
+        <v>43631</v>
+      </c>
+      <c r="F44" s="140"/>
+      <c r="G44" s="140"/>
+      <c r="H44" s="140"/>
+      <c r="I44" s="140"/>
+      <c r="J44" s="158"/>
+      <c r="K44" s="157"/>
+      <c r="L44" s="140"/>
+      <c r="M44" s="153"/>
+      <c r="N44" s="153"/>
+      <c r="O44" s="153"/>
+      <c r="P44" s="153"/>
+      <c r="Q44" s="153"/>
+      <c r="R44" s="153"/>
+      <c r="S44" s="153"/>
+      <c r="T44" s="153"/>
     </row>
     <row r="45" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="87" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="B45" s="75" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C45" s="32"/>
       <c r="D45" s="67">
-        <f>D42+5</f>
-        <v>43626</v>
+        <f>E44+1</f>
+        <v>43632</v>
       </c>
       <c r="E45" s="67">
-        <f>D45+5</f>
-        <v>43631</v>
-      </c>
-      <c r="F45" s="116"/>
-      <c r="G45" s="116"/>
-      <c r="H45" s="116"/>
-      <c r="I45" s="116"/>
-      <c r="J45" s="117"/>
-      <c r="K45" s="116"/>
-      <c r="L45" s="116"/>
-      <c r="M45" s="116"/>
-      <c r="N45" s="116"/>
-      <c r="O45" s="116"/>
-      <c r="P45" s="116"/>
-      <c r="Q45" s="116"/>
-      <c r="R45" s="116"/>
-      <c r="S45" s="116"/>
-      <c r="T45" s="116"/>
+        <f>D45+4</f>
+        <v>43636</v>
+      </c>
+      <c r="F45" s="140"/>
+      <c r="G45" s="140"/>
+      <c r="H45" s="140"/>
+      <c r="I45" s="140"/>
+      <c r="J45" s="158"/>
+      <c r="K45" s="157"/>
+      <c r="L45" s="153"/>
+      <c r="M45" s="153"/>
+      <c r="N45" s="153"/>
+      <c r="O45" s="153"/>
+      <c r="P45" s="153"/>
+      <c r="Q45" s="153"/>
+      <c r="R45" s="153"/>
+      <c r="S45" s="153"/>
+      <c r="T45" s="153"/>
     </row>
     <row r="46" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="87" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" s="75" t="s">
-        <v>133</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="B46" s="75"/>
       <c r="C46" s="32"/>
       <c r="D46" s="67">
-        <f>E45+1</f>
-        <v>43632</v>
+        <f>D44</f>
+        <v>43626</v>
       </c>
       <c r="E46" s="67">
         <f>D46+4</f>
-        <v>43636</v>
-      </c>
-      <c r="F46" s="116"/>
-      <c r="G46" s="116"/>
-      <c r="H46" s="116"/>
-      <c r="I46" s="116"/>
-      <c r="J46" s="117"/>
-      <c r="K46" s="116"/>
-      <c r="L46" s="116"/>
-      <c r="M46" s="116"/>
-      <c r="N46" s="116"/>
-      <c r="O46" s="116"/>
-      <c r="P46" s="116"/>
-      <c r="Q46" s="116"/>
-      <c r="R46" s="116"/>
-      <c r="S46" s="116"/>
-      <c r="T46" s="116"/>
+        <v>43630</v>
+      </c>
+      <c r="F46" s="140"/>
+      <c r="G46" s="140"/>
+      <c r="H46" s="140"/>
+      <c r="I46" s="140"/>
+      <c r="J46" s="158"/>
+      <c r="K46" s="170"/>
+      <c r="L46" s="153"/>
+      <c r="M46" s="153"/>
+      <c r="N46" s="153"/>
+      <c r="O46" s="153"/>
+      <c r="P46" s="153"/>
+      <c r="Q46" s="140"/>
+      <c r="R46" s="140"/>
+      <c r="S46" s="140"/>
+      <c r="T46" s="140"/>
     </row>
     <row r="47" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="87" t="s">
+      <c r="A47" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B47" s="76"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="154"/>
+      <c r="G47" s="154"/>
+      <c r="H47" s="154"/>
+      <c r="I47" s="154"/>
+      <c r="J47" s="155"/>
+      <c r="K47" s="154"/>
+      <c r="L47" s="154"/>
+      <c r="M47" s="154"/>
+      <c r="N47" s="154"/>
+      <c r="O47" s="154"/>
+      <c r="P47" s="154"/>
+      <c r="Q47" s="154"/>
+      <c r="R47" s="154"/>
+      <c r="S47" s="154"/>
+      <c r="T47" s="154"/>
+    </row>
+    <row r="48" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="79" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="75"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="67">
-        <f>D45</f>
-        <v>43626</v>
-      </c>
-      <c r="E47" s="67">
-        <f>D47+4</f>
-        <v>43630</v>
-      </c>
-      <c r="F47" s="116"/>
-      <c r="G47" s="116"/>
-      <c r="H47" s="116"/>
-      <c r="I47" s="116"/>
-      <c r="J47" s="117"/>
-      <c r="K47" s="116"/>
-      <c r="L47" s="116"/>
-      <c r="M47" s="116"/>
-      <c r="N47" s="116"/>
-      <c r="O47" s="116"/>
-      <c r="P47" s="116"/>
-      <c r="Q47" s="116"/>
-      <c r="R47" s="116"/>
-      <c r="S47" s="116"/>
-      <c r="T47" s="116"/>
-    </row>
-    <row r="48" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="B48" s="76"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="76"/>
-      <c r="G48" s="76"/>
-      <c r="H48" s="76"/>
-      <c r="I48" s="76"/>
-      <c r="J48" s="76"/>
-      <c r="K48" s="76"/>
-      <c r="L48" s="76"/>
-      <c r="M48" s="76"/>
-      <c r="N48" s="76"/>
-      <c r="O48" s="76"/>
-      <c r="P48" s="76"/>
-      <c r="Q48" s="76"/>
-      <c r="R48" s="76"/>
-      <c r="S48" s="76"/>
-      <c r="T48" s="76"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="F48" s="140"/>
+      <c r="G48" s="140"/>
+      <c r="H48" s="140"/>
+      <c r="I48" s="140"/>
+      <c r="J48" s="158"/>
+      <c r="K48" s="157"/>
+      <c r="L48" s="140"/>
+      <c r="M48" s="140"/>
+      <c r="N48" s="140"/>
+      <c r="O48" s="140"/>
+      <c r="P48" s="156"/>
+      <c r="Q48" s="156"/>
+      <c r="R48" s="156"/>
+      <c r="S48" s="156"/>
+      <c r="T48" s="156"/>
     </row>
     <row r="49" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="79" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B49" s="77" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C49" s="37"/>
       <c r="D49" s="68" t="s">
@@ -7371,25 +7755,25 @@
       <c r="E49" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="F49" s="116"/>
-      <c r="G49" s="116"/>
-      <c r="H49" s="116"/>
-      <c r="I49" s="116"/>
-      <c r="J49" s="117"/>
-      <c r="K49" s="116"/>
-      <c r="L49" s="116"/>
-      <c r="M49" s="116"/>
-      <c r="N49" s="116"/>
-      <c r="O49" s="116"/>
-      <c r="P49" s="116"/>
-      <c r="Q49" s="116"/>
-      <c r="R49" s="116"/>
-      <c r="S49" s="116"/>
-      <c r="T49" s="116"/>
+      <c r="F49" s="140"/>
+      <c r="G49" s="140"/>
+      <c r="H49" s="140"/>
+      <c r="I49" s="140"/>
+      <c r="J49" s="158"/>
+      <c r="K49" s="157"/>
+      <c r="L49" s="140"/>
+      <c r="M49" s="140"/>
+      <c r="N49" s="140"/>
+      <c r="O49" s="140"/>
+      <c r="P49" s="156"/>
+      <c r="Q49" s="156"/>
+      <c r="R49" s="156"/>
+      <c r="S49" s="156"/>
+      <c r="T49" s="156"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="79" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B50" s="77" t="s">
         <v>137</v>
@@ -7401,29 +7785,27 @@
       <c r="E50" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="F50" s="116"/>
-      <c r="G50" s="116"/>
-      <c r="H50" s="116"/>
-      <c r="I50" s="116"/>
-      <c r="J50" s="117"/>
-      <c r="K50" s="116"/>
-      <c r="L50" s="116"/>
-      <c r="M50" s="116"/>
-      <c r="N50" s="116"/>
-      <c r="O50" s="116"/>
-      <c r="P50" s="116"/>
-      <c r="Q50" s="116"/>
-      <c r="R50" s="116"/>
-      <c r="S50" s="116"/>
-      <c r="T50" s="116"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="140"/>
+      <c r="H50" s="140"/>
+      <c r="I50" s="140"/>
+      <c r="J50" s="158"/>
+      <c r="K50" s="157"/>
+      <c r="L50" s="140"/>
+      <c r="M50" s="140"/>
+      <c r="N50" s="140"/>
+      <c r="O50" s="140"/>
+      <c r="P50" s="156"/>
+      <c r="Q50" s="156"/>
+      <c r="R50" s="156"/>
+      <c r="S50" s="156"/>
+      <c r="T50" s="156"/>
     </row>
     <row r="51" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="79" t="s">
-        <v>139</v>
-      </c>
-      <c r="B51" s="77" t="s">
-        <v>140</v>
-      </c>
+      <c r="A51" s="117" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="77"/>
       <c r="C51" s="37"/>
       <c r="D51" s="68" t="s">
         <v>31</v>
@@ -7431,25 +7813,25 @@
       <c r="E51" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="F51" s="116"/>
-      <c r="G51" s="116"/>
-      <c r="H51" s="116"/>
-      <c r="I51" s="116"/>
-      <c r="J51" s="117"/>
-      <c r="K51" s="116"/>
-      <c r="L51" s="116"/>
-      <c r="M51" s="116"/>
-      <c r="N51" s="116"/>
-      <c r="O51" s="116"/>
-      <c r="P51" s="116"/>
-      <c r="Q51" s="116"/>
-      <c r="R51" s="116"/>
-      <c r="S51" s="116"/>
-      <c r="T51" s="116"/>
+      <c r="F51" s="140"/>
+      <c r="G51" s="140"/>
+      <c r="H51" s="140"/>
+      <c r="I51" s="140"/>
+      <c r="J51" s="158"/>
+      <c r="K51" s="157"/>
+      <c r="L51" s="140"/>
+      <c r="M51" s="140"/>
+      <c r="N51" s="140"/>
+      <c r="O51" s="140"/>
+      <c r="P51" s="156"/>
+      <c r="Q51" s="156"/>
+      <c r="R51" s="156"/>
+      <c r="S51" s="156"/>
+      <c r="T51" s="156"/>
     </row>
     <row r="52" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="139" t="s">
-        <v>1</v>
+      <c r="A52" s="117" t="s">
+        <v>2</v>
       </c>
       <c r="B52" s="77"/>
       <c r="C52" s="37"/>
@@ -7459,59 +7841,31 @@
       <c r="E52" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="F52" s="116"/>
-      <c r="G52" s="116"/>
-      <c r="H52" s="116"/>
-      <c r="I52" s="116"/>
-      <c r="J52" s="117"/>
-      <c r="K52" s="116"/>
-      <c r="L52" s="116"/>
-      <c r="M52" s="116"/>
-      <c r="N52" s="116"/>
-      <c r="O52" s="116"/>
-      <c r="P52" s="116"/>
-      <c r="Q52" s="116"/>
-      <c r="R52" s="116"/>
-      <c r="S52" s="116"/>
-      <c r="T52" s="116"/>
-    </row>
-    <row r="53" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B53" s="77"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="E53" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="F53" s="116"/>
-      <c r="G53" s="116"/>
-      <c r="H53" s="116"/>
-      <c r="I53" s="116"/>
-      <c r="J53" s="117"/>
-      <c r="K53" s="116"/>
-      <c r="L53" s="116"/>
-      <c r="M53" s="116"/>
-      <c r="N53" s="116"/>
-      <c r="O53" s="116"/>
-      <c r="P53" s="116"/>
-      <c r="Q53" s="116"/>
-      <c r="R53" s="116"/>
-      <c r="S53" s="116"/>
-      <c r="T53" s="116"/>
+      <c r="F52" s="140"/>
+      <c r="G52" s="140"/>
+      <c r="H52" s="140"/>
+      <c r="I52" s="140"/>
+      <c r="J52" s="158"/>
+      <c r="K52" s="157"/>
+      <c r="L52" s="140"/>
+      <c r="M52" s="140"/>
+      <c r="N52" s="140"/>
+      <c r="O52" s="140"/>
+      <c r="P52" s="156"/>
+      <c r="Q52" s="156"/>
+      <c r="R52" s="156"/>
+      <c r="S52" s="156"/>
+      <c r="T52" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
-  <conditionalFormatting sqref="C7:C53">
-    <cfRule type="dataBar" priority="4">
+  <conditionalFormatting sqref="C6:C52">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7524,8 +7878,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8:T8">
-    <cfRule type="dataBar" priority="3">
+  <conditionalFormatting sqref="F7:T7">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7538,8 +7892,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28:T28">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="F27:T27">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7552,8 +7906,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39:T39">
-    <cfRule type="dataBar" priority="1">
+  <conditionalFormatting sqref="F38:T38">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7566,12 +7920,22 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="D4" xr:uid="{3DD3FEA8-6A82-4281-9AA6-17B0161617BC}">
-      <formula1>1</formula1>
-    </dataValidation>
-  </dataValidations>
+  <conditionalFormatting sqref="U7">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E9C65209-3DCB-4717-98EB-3D9411BE612B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -7588,7 +7952,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C7:C53</xm:sqref>
+          <xm:sqref>C6:C52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{92EF9621-5146-4436-BCF1-461ED7DC6BAF}">
@@ -7603,7 +7967,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F8:T8</xm:sqref>
+          <xm:sqref>F7:T7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{AFDD33DB-9CC4-4288-AC6B-AD988108A30E}">
@@ -7618,7 +7982,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F28:T28</xm:sqref>
+          <xm:sqref>F27:T27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{60D034B9-2641-44A8-A5DE-B373777B8A30}">
@@ -7633,7 +7997,22 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F39:T39</xm:sqref>
+          <xm:sqref>F38:T38</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E9C65209-3DCB-4717-98EB-3D9411BE612B}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>U7</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
minor corrections, new pdf
</commit_message>
<xml_diff>
--- a/Assignment 3 timeframe..xlsx
+++ b/Assignment 3 timeframe..xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EB7C99-50DB-44AE-8C83-6D424E04C05D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1053F4-5F3B-46DB-B2E0-22CEC48DBDD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20052" yWindow="4092" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -741,7 +741,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -877,6 +877,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1331,7 +1343,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="196">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1651,43 +1663,7 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="18" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="13" xfId="9" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="14" xfId="9" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1751,12 +1727,6 @@
     <xf numFmtId="165" fontId="5" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1794,12 +1764,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="2" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="10" borderId="2" xfId="11" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1831,9 +1795,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="18" borderId="17" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="2" xfId="11" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="24" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1843,9 +1804,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1854,6 +1812,78 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="13" xfId="9" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="14" xfId="9" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="24" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="24" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="24" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="2" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -2476,14 +2506,14 @@
       <c r="B3" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="180" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="120"/>
-      <c r="E3" s="128">
+      <c r="D3" s="181"/>
+      <c r="E3" s="179">
         <v>43570</v>
       </c>
-      <c r="F3" s="128"/>
+      <c r="F3" s="179"/>
       <c r="I3">
         <v>1</v>
       </c>
@@ -2495,104 +2525,104 @@
       <c r="B4" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="119" t="s">
+      <c r="C4" s="180" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="120"/>
+      <c r="D4" s="181"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="125">
+      <c r="I4" s="176">
         <f>I5</f>
         <v>43570</v>
       </c>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="126"/>
-      <c r="M4" s="126"/>
-      <c r="N4" s="126"/>
-      <c r="O4" s="127"/>
-      <c r="P4" s="125">
+      <c r="J4" s="177"/>
+      <c r="K4" s="177"/>
+      <c r="L4" s="177"/>
+      <c r="M4" s="177"/>
+      <c r="N4" s="177"/>
+      <c r="O4" s="178"/>
+      <c r="P4" s="176">
         <f>P5</f>
         <v>43577</v>
       </c>
-      <c r="Q4" s="126"/>
-      <c r="R4" s="126"/>
-      <c r="S4" s="126"/>
-      <c r="T4" s="126"/>
-      <c r="U4" s="126"/>
-      <c r="V4" s="127"/>
-      <c r="W4" s="125">
+      <c r="Q4" s="177"/>
+      <c r="R4" s="177"/>
+      <c r="S4" s="177"/>
+      <c r="T4" s="177"/>
+      <c r="U4" s="177"/>
+      <c r="V4" s="178"/>
+      <c r="W4" s="176">
         <f>W5</f>
         <v>43584</v>
       </c>
-      <c r="X4" s="126"/>
-      <c r="Y4" s="126"/>
-      <c r="Z4" s="126"/>
-      <c r="AA4" s="126"/>
-      <c r="AB4" s="126"/>
-      <c r="AC4" s="127"/>
-      <c r="AD4" s="125">
+      <c r="X4" s="177"/>
+      <c r="Y4" s="177"/>
+      <c r="Z4" s="177"/>
+      <c r="AA4" s="177"/>
+      <c r="AB4" s="177"/>
+      <c r="AC4" s="178"/>
+      <c r="AD4" s="176">
         <f>AD5</f>
         <v>43591</v>
       </c>
-      <c r="AE4" s="126"/>
-      <c r="AF4" s="126"/>
-      <c r="AG4" s="126"/>
-      <c r="AH4" s="126"/>
-      <c r="AI4" s="126"/>
-      <c r="AJ4" s="127"/>
-      <c r="AK4" s="122">
+      <c r="AE4" s="177"/>
+      <c r="AF4" s="177"/>
+      <c r="AG4" s="177"/>
+      <c r="AH4" s="177"/>
+      <c r="AI4" s="177"/>
+      <c r="AJ4" s="178"/>
+      <c r="AK4" s="183">
         <f>AK5</f>
         <v>43598</v>
       </c>
-      <c r="AL4" s="123"/>
-      <c r="AM4" s="123"/>
-      <c r="AN4" s="123"/>
-      <c r="AO4" s="123"/>
-      <c r="AP4" s="123"/>
-      <c r="AQ4" s="124"/>
-      <c r="AR4" s="125">
+      <c r="AL4" s="184"/>
+      <c r="AM4" s="184"/>
+      <c r="AN4" s="184"/>
+      <c r="AO4" s="184"/>
+      <c r="AP4" s="184"/>
+      <c r="AQ4" s="185"/>
+      <c r="AR4" s="176">
         <f>AR5</f>
         <v>43605</v>
       </c>
-      <c r="AS4" s="126"/>
-      <c r="AT4" s="126"/>
-      <c r="AU4" s="126"/>
-      <c r="AV4" s="126"/>
-      <c r="AW4" s="126"/>
-      <c r="AX4" s="127"/>
-      <c r="AY4" s="125">
+      <c r="AS4" s="177"/>
+      <c r="AT4" s="177"/>
+      <c r="AU4" s="177"/>
+      <c r="AV4" s="177"/>
+      <c r="AW4" s="177"/>
+      <c r="AX4" s="178"/>
+      <c r="AY4" s="176">
         <f>AY5</f>
         <v>43612</v>
       </c>
-      <c r="AZ4" s="126"/>
-      <c r="BA4" s="126"/>
-      <c r="BB4" s="126"/>
-      <c r="BC4" s="126"/>
-      <c r="BD4" s="126"/>
-      <c r="BE4" s="127"/>
-      <c r="BF4" s="125">
+      <c r="AZ4" s="177"/>
+      <c r="BA4" s="177"/>
+      <c r="BB4" s="177"/>
+      <c r="BC4" s="177"/>
+      <c r="BD4" s="177"/>
+      <c r="BE4" s="178"/>
+      <c r="BF4" s="176">
         <f>BF5</f>
         <v>43619</v>
       </c>
-      <c r="BG4" s="126"/>
-      <c r="BH4" s="126"/>
-      <c r="BI4" s="126"/>
-      <c r="BJ4" s="126"/>
-      <c r="BK4" s="126"/>
-      <c r="BL4" s="127"/>
+      <c r="BG4" s="177"/>
+      <c r="BH4" s="177"/>
+      <c r="BI4" s="177"/>
+      <c r="BJ4" s="177"/>
+      <c r="BK4" s="177"/>
+      <c r="BL4" s="178"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="121"/>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="121"/>
-      <c r="G5" s="121"/>
+      <c r="B5" s="182"/>
+      <c r="C5" s="182"/>
+      <c r="D5" s="182"/>
+      <c r="E5" s="182"/>
+      <c r="F5" s="182"/>
+      <c r="G5" s="182"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43570</v>
@@ -6328,6 +6358,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -6335,11 +6370,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D49">
     <cfRule type="dataBar" priority="14">
@@ -6518,8 +6548,8 @@
   <dimension ref="A1:U52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:U52"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6533,29 +6563,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="149" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="168"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="171"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
-      <c r="P1" s="170"/>
-      <c r="Q1" s="170"/>
-      <c r="R1" s="170"/>
-      <c r="S1" s="170"/>
-      <c r="T1" s="170"/>
-      <c r="U1" s="170"/>
+      <c r="B1" s="150"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="155"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
+      <c r="P1" s="154"/>
+      <c r="Q1" s="154"/>
+      <c r="R1" s="154"/>
+      <c r="S1" s="154"/>
+      <c r="T1" s="154"/>
+      <c r="U1" s="154"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="89" t="s">
@@ -6563,16 +6593,16 @@
       </c>
       <c r="B2" s="89"/>
       <c r="C2" s="89"/>
-      <c r="D2" s="129">
+      <c r="D2" s="186">
         <v>43570</v>
       </c>
-      <c r="E2" s="130"/>
+      <c r="E2" s="187"/>
       <c r="G2" s="88"/>
       <c r="H2" s="88"/>
-      <c r="I2" s="160" t="s">
+      <c r="I2" s="188" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="159" t="s">
+      <c r="J2" s="189" t="s">
         <v>109</v>
       </c>
       <c r="K2" s="88"/>
@@ -6594,8 +6624,8 @@
       <c r="C3" s="102"/>
       <c r="D3" s="102"/>
       <c r="E3" s="102"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="159"/>
+      <c r="I3" s="188"/>
+      <c r="J3" s="189"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="102"/>
@@ -6603,52 +6633,52 @@
       <c r="C4" s="102"/>
       <c r="D4" s="102"/>
       <c r="E4" s="102"/>
-      <c r="F4" s="190">
+      <c r="F4" s="171">
         <v>43570</v>
       </c>
-      <c r="G4" s="190">
+      <c r="G4" s="171">
         <v>43577</v>
       </c>
-      <c r="H4" s="190">
+      <c r="H4" s="171">
         <v>43584</v>
       </c>
-      <c r="I4" s="190">
+      <c r="I4" s="171">
         <v>43591</v>
       </c>
-      <c r="J4" s="191">
+      <c r="J4" s="172">
         <v>43598</v>
       </c>
-      <c r="K4" s="190">
+      <c r="K4" s="171">
         <v>43605</v>
       </c>
-      <c r="L4" s="190">
+      <c r="L4" s="171">
         <v>43612</v>
       </c>
-      <c r="M4" s="190">
+      <c r="M4" s="171">
         <v>43619</v>
       </c>
-      <c r="N4" s="190">
+      <c r="N4" s="171">
         <v>43626</v>
       </c>
-      <c r="O4" s="190">
+      <c r="O4" s="171">
         <v>43633</v>
       </c>
-      <c r="P4" s="190">
+      <c r="P4" s="171">
         <v>43640</v>
       </c>
-      <c r="Q4" s="190">
+      <c r="Q4" s="171">
         <v>43647</v>
       </c>
-      <c r="R4" s="190">
+      <c r="R4" s="171">
         <v>43654</v>
       </c>
-      <c r="S4" s="190">
+      <c r="S4" s="171">
         <v>43661</v>
       </c>
-      <c r="T4" s="190">
+      <c r="T4" s="171">
         <v>43668</v>
       </c>
-      <c r="U4" s="192" t="s">
+      <c r="U4" s="190" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6668,52 +6698,52 @@
       <c r="E5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="193" t="s">
+      <c r="F5" s="173" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="193" t="s">
+      <c r="G5" s="173" t="s">
         <v>92</v>
       </c>
-      <c r="H5" s="193" t="s">
+      <c r="H5" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I5" s="193" t="s">
+      <c r="I5" s="173" t="s">
         <v>94</v>
       </c>
-      <c r="J5" s="194" t="s">
+      <c r="J5" s="174" t="s">
         <v>95</v>
       </c>
-      <c r="K5" s="193" t="s">
+      <c r="K5" s="173" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="193" t="s">
+      <c r="L5" s="173" t="s">
         <v>97</v>
       </c>
-      <c r="M5" s="193" t="s">
+      <c r="M5" s="173" t="s">
         <v>98</v>
       </c>
-      <c r="N5" s="193" t="s">
+      <c r="N5" s="173" t="s">
         <v>99</v>
       </c>
-      <c r="O5" s="193" t="s">
+      <c r="O5" s="173" t="s">
         <v>100</v>
       </c>
-      <c r="P5" s="193" t="s">
+      <c r="P5" s="173" t="s">
         <v>101</v>
       </c>
-      <c r="Q5" s="193" t="s">
+      <c r="Q5" s="173" t="s">
         <v>102</v>
       </c>
-      <c r="R5" s="193" t="s">
+      <c r="R5" s="173" t="s">
         <v>103</v>
       </c>
-      <c r="S5" s="193" t="s">
+      <c r="S5" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="T5" s="193" t="s">
+      <c r="T5" s="173" t="s">
         <v>105</v>
       </c>
-      <c r="U5" s="192"/>
+      <c r="U5" s="190"/>
     </row>
     <row r="6" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="90" t="s">
@@ -6721,67 +6751,67 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="154" t="s">
+      <c r="A7" s="140" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="155"/>
-      <c r="C7" s="156"/>
-      <c r="D7" s="157"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="156"/>
-      <c r="H7" s="156"/>
-      <c r="I7" s="156"/>
-      <c r="J7" s="156"/>
-      <c r="K7" s="156"/>
-      <c r="L7" s="156"/>
-      <c r="M7" s="156"/>
-      <c r="N7" s="156"/>
-      <c r="O7" s="156"/>
-      <c r="P7" s="156"/>
-      <c r="Q7" s="156"/>
-      <c r="R7" s="156"/>
-      <c r="S7" s="156"/>
-      <c r="T7" s="156"/>
-      <c r="U7" s="156"/>
+      <c r="B7" s="141"/>
+      <c r="C7" s="142"/>
+      <c r="D7" s="143"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="142"/>
+      <c r="G7" s="142"/>
+      <c r="H7" s="142"/>
+      <c r="I7" s="142"/>
+      <c r="J7" s="142"/>
+      <c r="K7" s="142"/>
+      <c r="L7" s="142"/>
+      <c r="M7" s="142"/>
+      <c r="N7" s="142"/>
+      <c r="O7" s="142"/>
+      <c r="P7" s="142"/>
+      <c r="Q7" s="142"/>
+      <c r="R7" s="142"/>
+      <c r="S7" s="142"/>
+      <c r="T7" s="142"/>
+      <c r="U7" s="142"/>
     </row>
     <row r="8" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="172" t="s">
+      <c r="A8" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="146" t="s">
+      <c r="B8" s="132" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="147">
+      <c r="C8" s="133">
         <v>1</v>
       </c>
-      <c r="D8" s="148">
+      <c r="D8" s="134">
         <f>Project_Start</f>
         <v>43570</v>
       </c>
-      <c r="E8" s="149">
+      <c r="E8" s="135">
         <f>D8+12</f>
         <v>43582</v>
       </c>
-      <c r="F8" s="150"/>
-      <c r="G8" s="150"/>
-      <c r="H8" s="150"/>
-      <c r="I8" s="151"/>
-      <c r="J8" s="152"/>
-      <c r="K8" s="153"/>
-      <c r="L8" s="151"/>
-      <c r="M8" s="151"/>
-      <c r="N8" s="151"/>
-      <c r="O8" s="151"/>
-      <c r="P8" s="151"/>
-      <c r="Q8" s="151"/>
-      <c r="R8" s="151"/>
-      <c r="S8" s="151"/>
-      <c r="T8" s="151"/>
-      <c r="U8" s="151"/>
+      <c r="F8" s="136"/>
+      <c r="G8" s="136"/>
+      <c r="H8" s="136"/>
+      <c r="I8" s="137"/>
+      <c r="J8" s="138"/>
+      <c r="K8" s="139"/>
+      <c r="L8" s="137"/>
+      <c r="M8" s="137"/>
+      <c r="N8" s="137"/>
+      <c r="O8" s="137"/>
+      <c r="P8" s="137"/>
+      <c r="Q8" s="137"/>
+      <c r="R8" s="137"/>
+      <c r="S8" s="137"/>
+      <c r="T8" s="137"/>
+      <c r="U8" s="137"/>
     </row>
     <row r="9" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="157" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="93" t="s">
@@ -6801,7 +6831,7 @@
       <c r="G9" s="105"/>
       <c r="H9" s="105"/>
       <c r="I9" s="104"/>
-      <c r="J9" s="161"/>
+      <c r="J9" s="145"/>
       <c r="K9" s="114"/>
       <c r="L9" s="104"/>
       <c r="M9" s="104"/>
@@ -6815,7 +6845,7 @@
       <c r="U9" s="104"/>
     </row>
     <row r="10" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="157" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="93" t="s">
@@ -6835,7 +6865,7 @@
       <c r="G10" s="104"/>
       <c r="H10" s="104"/>
       <c r="I10" s="104"/>
-      <c r="J10" s="161"/>
+      <c r="J10" s="145"/>
       <c r="K10" s="114"/>
       <c r="L10" s="104"/>
       <c r="M10" s="104"/>
@@ -6849,7 +6879,7 @@
       <c r="U10" s="104"/>
     </row>
     <row r="11" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="157" t="s">
         <v>59</v>
       </c>
       <c r="B11" s="94" t="s">
@@ -6869,7 +6899,7 @@
       <c r="G11" s="104"/>
       <c r="H11" s="104"/>
       <c r="I11" s="104"/>
-      <c r="J11" s="179" t="s">
+      <c r="J11" s="161" t="s">
         <v>112</v>
       </c>
       <c r="K11" s="114"/>
@@ -6885,7 +6915,7 @@
       <c r="U11" s="104"/>
     </row>
     <row r="12" spans="1:21" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="173" t="s">
+      <c r="A12" s="157" t="s">
         <v>62</v>
       </c>
       <c r="B12" s="95" t="s">
@@ -6906,7 +6936,7 @@
       <c r="G12" s="106"/>
       <c r="H12" s="106"/>
       <c r="I12" s="104"/>
-      <c r="J12" s="161"/>
+      <c r="J12" s="145"/>
       <c r="K12" s="114"/>
       <c r="L12" s="104"/>
       <c r="M12" s="104"/>
@@ -6920,7 +6950,7 @@
       <c r="U12" s="104"/>
     </row>
     <row r="13" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="173" t="s">
+      <c r="A13" s="157" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="95" t="s">
@@ -6940,7 +6970,7 @@
       <c r="G13" s="106"/>
       <c r="H13" s="106"/>
       <c r="I13" s="106"/>
-      <c r="J13" s="161"/>
+      <c r="J13" s="145"/>
       <c r="K13" s="114"/>
       <c r="L13" s="104"/>
       <c r="M13" s="104"/>
@@ -6954,7 +6984,7 @@
       <c r="U13" s="104"/>
     </row>
     <row r="14" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="157" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="93" t="s">
@@ -6974,7 +7004,7 @@
       <c r="G14" s="104"/>
       <c r="H14" s="104"/>
       <c r="I14" s="104"/>
-      <c r="J14" s="161"/>
+      <c r="J14" s="145"/>
       <c r="K14" s="114"/>
       <c r="L14" s="104"/>
       <c r="M14" s="104"/>
@@ -6988,7 +7018,7 @@
       <c r="U14" s="104"/>
     </row>
     <row r="15" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="173" t="s">
+      <c r="A15" s="157" t="s">
         <v>56</v>
       </c>
       <c r="B15" s="95" t="s">
@@ -7009,7 +7039,7 @@
       <c r="G15" s="106"/>
       <c r="H15" s="106"/>
       <c r="I15" s="106"/>
-      <c r="J15" s="180" t="s">
+      <c r="J15" s="162" t="s">
         <v>112</v>
       </c>
       <c r="K15" s="114"/>
@@ -7025,7 +7055,7 @@
       <c r="U15" s="104"/>
     </row>
     <row r="16" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="173" t="s">
+      <c r="A16" s="157" t="s">
         <v>63</v>
       </c>
       <c r="B16" s="96" t="s">
@@ -7046,7 +7076,7 @@
       <c r="G16" s="105"/>
       <c r="H16" s="105"/>
       <c r="I16" s="104"/>
-      <c r="J16" s="181"/>
+      <c r="J16" s="163"/>
       <c r="K16" s="114"/>
       <c r="L16" s="104"/>
       <c r="M16" s="104"/>
@@ -7060,7 +7090,7 @@
       <c r="U16" s="104"/>
     </row>
     <row r="17" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="173" t="s">
+      <c r="A17" s="157" t="s">
         <v>65</v>
       </c>
       <c r="B17" s="97" t="s">
@@ -7075,7 +7105,7 @@
       <c r="G17" s="107"/>
       <c r="H17" s="107"/>
       <c r="I17" s="104"/>
-      <c r="J17" s="181"/>
+      <c r="J17" s="163"/>
       <c r="K17" s="114"/>
       <c r="L17" s="104"/>
       <c r="M17" s="104"/>
@@ -7089,7 +7119,7 @@
       <c r="U17" s="104"/>
     </row>
     <row r="18" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="173" t="s">
+      <c r="A18" s="157" t="s">
         <v>66</v>
       </c>
       <c r="B18" s="97" t="s">
@@ -7104,7 +7134,7 @@
       <c r="G18" s="104"/>
       <c r="H18" s="107"/>
       <c r="I18" s="107"/>
-      <c r="J18" s="181"/>
+      <c r="J18" s="163"/>
       <c r="K18" s="114"/>
       <c r="L18" s="104"/>
       <c r="M18" s="104"/>
@@ -7118,7 +7148,7 @@
       <c r="U18" s="104"/>
     </row>
     <row r="19" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="173" t="s">
+      <c r="A19" s="157" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="99" t="s">
@@ -7139,7 +7169,7 @@
       <c r="G19" s="108"/>
       <c r="H19" s="108"/>
       <c r="I19" s="108"/>
-      <c r="J19" s="179" t="s">
+      <c r="J19" s="161" t="s">
         <v>112</v>
       </c>
       <c r="K19" s="114"/>
@@ -7155,7 +7185,7 @@
       <c r="U19" s="104"/>
     </row>
     <row r="20" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="173" t="s">
+      <c r="A20" s="157" t="s">
         <v>69</v>
       </c>
       <c r="B20" s="98" t="s">
@@ -7176,7 +7206,7 @@
       <c r="G20" s="109"/>
       <c r="H20" s="104"/>
       <c r="I20" s="104"/>
-      <c r="J20" s="181"/>
+      <c r="J20" s="163"/>
       <c r="K20" s="114"/>
       <c r="L20" s="104"/>
       <c r="M20" s="104"/>
@@ -7190,7 +7220,7 @@
       <c r="U20" s="104"/>
     </row>
     <row r="21" spans="1:21" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="173" t="s">
+      <c r="A21" s="157" t="s">
         <v>71</v>
       </c>
       <c r="B21" s="99" t="s">
@@ -7205,7 +7235,7 @@
       <c r="G21" s="104"/>
       <c r="H21" s="104"/>
       <c r="I21" s="104"/>
-      <c r="J21" s="181"/>
+      <c r="J21" s="163"/>
       <c r="K21" s="114"/>
       <c r="L21" s="104"/>
       <c r="M21" s="104"/>
@@ -7219,7 +7249,7 @@
       <c r="U21" s="104"/>
     </row>
     <row r="22" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="173" t="s">
+      <c r="A22" s="157" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="100" t="s">
@@ -7240,7 +7270,7 @@
       <c r="G22" s="110"/>
       <c r="H22" s="110"/>
       <c r="I22" s="104"/>
-      <c r="J22" s="181"/>
+      <c r="J22" s="163"/>
       <c r="K22" s="114"/>
       <c r="L22" s="104"/>
       <c r="M22" s="104"/>
@@ -7254,7 +7284,7 @@
       <c r="U22" s="104"/>
     </row>
     <row r="23" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="173" t="s">
+      <c r="A23" s="157" t="s">
         <v>145</v>
       </c>
       <c r="B23" s="99" t="s">
@@ -7274,7 +7304,7 @@
       <c r="G23" s="104"/>
       <c r="H23" s="104"/>
       <c r="I23" s="108"/>
-      <c r="J23" s="179" t="s">
+      <c r="J23" s="161" t="s">
         <v>112</v>
       </c>
       <c r="K23" s="114"/>
@@ -7290,7 +7320,7 @@
       <c r="U23" s="104"/>
     </row>
     <row r="24" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="173" t="s">
+      <c r="A24" s="157" t="s">
         <v>116</v>
       </c>
       <c r="B24" s="98" t="s">
@@ -7308,11 +7338,11 @@
       </c>
       <c r="F24" s="111"/>
       <c r="G24" s="111"/>
-      <c r="H24" s="162" t="s">
+      <c r="H24" s="146" t="s">
         <v>112</v>
       </c>
       <c r="I24" s="104"/>
-      <c r="J24" s="181"/>
+      <c r="J24" s="163"/>
       <c r="K24" s="114"/>
       <c r="L24" s="104"/>
       <c r="M24" s="104"/>
@@ -7326,7 +7356,7 @@
       <c r="U24" s="104"/>
     </row>
     <row r="25" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="174" t="s">
+      <c r="A25" s="158" t="s">
         <v>75</v>
       </c>
       <c r="B25" s="98" t="s">
@@ -7346,7 +7376,7 @@
       <c r="G25" s="104"/>
       <c r="H25" s="104"/>
       <c r="I25" s="111"/>
-      <c r="J25" s="182" t="s">
+      <c r="J25" s="164" t="s">
         <v>112</v>
       </c>
       <c r="K25" s="114"/>
@@ -7362,71 +7392,71 @@
       <c r="U25" s="104"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="175" t="s">
+      <c r="A26" s="159" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="134" t="s">
+      <c r="B26" s="120" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="135">
+      <c r="C26" s="121">
         <v>1</v>
       </c>
-      <c r="D26" s="136">
+      <c r="D26" s="122">
         <v>43604</v>
       </c>
-      <c r="E26" s="137">
+      <c r="E26" s="123">
         <f>D26</f>
         <v>43604</v>
       </c>
-      <c r="F26" s="138"/>
-      <c r="G26" s="138"/>
-      <c r="H26" s="138"/>
-      <c r="I26" s="139"/>
-      <c r="J26" s="183" t="s">
+      <c r="F26" s="124"/>
+      <c r="G26" s="124"/>
+      <c r="H26" s="124"/>
+      <c r="I26" s="125"/>
+      <c r="J26" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="K26" s="140"/>
-      <c r="L26" s="138"/>
-      <c r="M26" s="138"/>
-      <c r="N26" s="138"/>
-      <c r="O26" s="138"/>
-      <c r="P26" s="138"/>
-      <c r="Q26" s="138"/>
-      <c r="R26" s="138"/>
-      <c r="S26" s="138"/>
-      <c r="T26" s="138"/>
-      <c r="U26" s="138"/>
+      <c r="K26" s="126"/>
+      <c r="L26" s="124"/>
+      <c r="M26" s="124"/>
+      <c r="N26" s="124"/>
+      <c r="O26" s="124"/>
+      <c r="P26" s="124"/>
+      <c r="Q26" s="124"/>
+      <c r="R26" s="124"/>
+      <c r="S26" s="124"/>
+      <c r="T26" s="124"/>
+      <c r="U26" s="124"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="141" t="s">
+      <c r="A27" s="127" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="142"/>
-      <c r="C27" s="142"/>
-      <c r="D27" s="142"/>
-      <c r="E27" s="142"/>
-      <c r="F27" s="142"/>
-      <c r="G27" s="142"/>
-      <c r="H27" s="142"/>
-      <c r="I27" s="142"/>
-      <c r="J27" s="184"/>
-      <c r="K27" s="142"/>
-      <c r="L27" s="142"/>
-      <c r="M27" s="142"/>
-      <c r="N27" s="142"/>
-      <c r="O27" s="142"/>
-      <c r="P27" s="142"/>
-      <c r="Q27" s="142"/>
-      <c r="R27" s="142"/>
-      <c r="S27" s="142"/>
-      <c r="T27" s="142"/>
-      <c r="U27" s="142"/>
+      <c r="B27" s="128"/>
+      <c r="C27" s="128"/>
+      <c r="D27" s="128"/>
+      <c r="E27" s="128"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="128"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="128"/>
+      <c r="J27" s="166"/>
+      <c r="K27" s="128"/>
+      <c r="L27" s="128"/>
+      <c r="M27" s="128"/>
+      <c r="N27" s="128"/>
+      <c r="O27" s="128"/>
+      <c r="P27" s="128"/>
+      <c r="Q27" s="128"/>
+      <c r="R27" s="128"/>
+      <c r="S27" s="128"/>
+      <c r="T27" s="128"/>
+      <c r="U27" s="128"/>
     </row>
     <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="86" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="145" t="s">
+      <c r="B28" s="131" t="s">
         <v>53</v>
       </c>
       <c r="C28" s="27">
@@ -7444,7 +7474,7 @@
       <c r="G28" s="106"/>
       <c r="H28" s="106"/>
       <c r="I28" s="104"/>
-      <c r="J28" s="181"/>
+      <c r="J28" s="163"/>
       <c r="K28" s="114"/>
       <c r="L28" s="104"/>
       <c r="M28" s="104"/>
@@ -7461,7 +7491,7 @@
       <c r="A29" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="145" t="s">
+      <c r="B29" s="131" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="27">
@@ -7479,7 +7509,7 @@
       <c r="G29" s="106"/>
       <c r="H29" s="106"/>
       <c r="I29" s="104"/>
-      <c r="J29" s="181"/>
+      <c r="J29" s="163"/>
       <c r="K29" s="114"/>
       <c r="L29" s="104"/>
       <c r="M29" s="104"/>
@@ -7496,7 +7526,7 @@
       <c r="A30" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="143" t="s">
+      <c r="B30" s="129" t="s">
         <v>115</v>
       </c>
       <c r="C30" s="27">
@@ -7508,7 +7538,7 @@
       <c r="G30" s="112"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
-      <c r="J30" s="181"/>
+      <c r="J30" s="163"/>
       <c r="K30" s="114"/>
       <c r="L30" s="104"/>
       <c r="M30" s="104"/>
@@ -7525,7 +7555,7 @@
       <c r="A31" s="86" t="s">
         <v>119</v>
       </c>
-      <c r="B31" s="145" t="s">
+      <c r="B31" s="131" t="s">
         <v>53</v>
       </c>
       <c r="C31" s="27"/>
@@ -7541,7 +7571,7 @@
       <c r="G31" s="104"/>
       <c r="H31" s="104"/>
       <c r="I31" s="104"/>
-      <c r="J31" s="181"/>
+      <c r="J31" s="163"/>
       <c r="K31" s="106"/>
       <c r="L31" s="106"/>
       <c r="M31" s="106"/>
@@ -7558,7 +7588,7 @@
       <c r="A32" s="86" t="s">
         <v>120</v>
       </c>
-      <c r="B32" s="143" t="s">
+      <c r="B32" s="129" t="s">
         <v>115</v>
       </c>
       <c r="C32" s="27"/>
@@ -7568,7 +7598,7 @@
       <c r="G32" s="104"/>
       <c r="H32" s="104"/>
       <c r="I32" s="104"/>
-      <c r="J32" s="181"/>
+      <c r="J32" s="163"/>
       <c r="K32" s="114"/>
       <c r="L32" s="104"/>
       <c r="M32" s="112"/>
@@ -7585,7 +7615,7 @@
       <c r="A33" s="86" t="s">
         <v>142</v>
       </c>
-      <c r="B33" s="145" t="s">
+      <c r="B33" s="131" t="s">
         <v>53</v>
       </c>
       <c r="C33" s="27">
@@ -7603,7 +7633,7 @@
       <c r="G33" s="104"/>
       <c r="H33" s="104"/>
       <c r="I33" s="106"/>
-      <c r="J33" s="181"/>
+      <c r="J33" s="163"/>
       <c r="K33" s="114"/>
       <c r="L33" s="104"/>
       <c r="M33" s="104"/>
@@ -7620,7 +7650,7 @@
       <c r="A34" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="143" t="s">
+      <c r="B34" s="129" t="s">
         <v>115</v>
       </c>
       <c r="C34" s="27"/>
@@ -7636,7 +7666,7 @@
       <c r="G34" s="104"/>
       <c r="H34" s="104"/>
       <c r="I34" s="112"/>
-      <c r="J34" s="185"/>
+      <c r="J34" s="167"/>
       <c r="K34" s="116"/>
       <c r="L34" s="112"/>
       <c r="M34" s="104"/>
@@ -7665,7 +7695,7 @@
       <c r="G35" s="110"/>
       <c r="H35" s="110"/>
       <c r="I35" s="110"/>
-      <c r="J35" s="186"/>
+      <c r="J35" s="168"/>
       <c r="K35" s="104"/>
       <c r="L35" s="104"/>
       <c r="M35" s="104"/>
@@ -7682,7 +7712,7 @@
       <c r="A36" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="144" t="s">
+      <c r="B36" s="130" t="s">
         <v>64</v>
       </c>
       <c r="C36" s="27">
@@ -7700,7 +7730,7 @@
       <c r="G36" s="104"/>
       <c r="H36" s="107"/>
       <c r="I36" s="107"/>
-      <c r="J36" s="187"/>
+      <c r="J36" s="169"/>
       <c r="K36" s="117"/>
       <c r="L36" s="107"/>
       <c r="M36" s="104"/>
@@ -7729,7 +7759,7 @@
       <c r="G37" s="113"/>
       <c r="H37" s="113"/>
       <c r="I37" s="113"/>
-      <c r="J37" s="188"/>
+      <c r="J37" s="170"/>
       <c r="K37" s="113"/>
       <c r="L37" s="104"/>
       <c r="M37" s="104"/>
@@ -7763,7 +7793,7 @@
       <c r="F38" s="104"/>
       <c r="G38" s="104"/>
       <c r="H38" s="104"/>
-      <c r="J38" s="181"/>
+      <c r="J38" s="163"/>
       <c r="K38" s="110"/>
       <c r="L38" s="110"/>
       <c r="M38" s="118"/>
@@ -7777,35 +7807,35 @@
       <c r="U38" s="104"/>
     </row>
     <row r="39" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="191" t="s">
         <v>122</v>
       </c>
-      <c r="B39" s="74"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="74"/>
-      <c r="G39" s="74"/>
-      <c r="H39" s="74"/>
-      <c r="I39" s="74"/>
-      <c r="J39" s="189"/>
-      <c r="K39" s="74"/>
-      <c r="L39" s="74"/>
-      <c r="M39" s="74"/>
-      <c r="N39" s="74"/>
-      <c r="O39" s="74"/>
-      <c r="P39" s="74"/>
-      <c r="Q39" s="74"/>
-      <c r="R39" s="74"/>
-      <c r="S39" s="74"/>
-      <c r="T39" s="74"/>
-      <c r="U39" s="74"/>
+      <c r="B39" s="192"/>
+      <c r="C39" s="193"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
+      <c r="F39" s="192"/>
+      <c r="G39" s="192"/>
+      <c r="H39" s="192"/>
+      <c r="I39" s="192"/>
+      <c r="J39" s="196"/>
+      <c r="K39" s="192"/>
+      <c r="L39" s="192"/>
+      <c r="M39" s="192"/>
+      <c r="N39" s="192"/>
+      <c r="O39" s="192"/>
+      <c r="P39" s="192"/>
+      <c r="Q39" s="192"/>
+      <c r="R39" s="192"/>
+      <c r="S39" s="192"/>
+      <c r="T39" s="192"/>
+      <c r="U39" s="192"/>
     </row>
     <row r="40" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="87" t="s">
+      <c r="A40" s="197" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="177" t="s">
+      <c r="B40" s="198" t="s">
         <v>123</v>
       </c>
       <c r="C40" s="32"/>
@@ -7821,24 +7851,24 @@
       <c r="G40" s="104"/>
       <c r="H40" s="104"/>
       <c r="I40" s="104"/>
-      <c r="J40" s="181"/>
-      <c r="K40" s="132"/>
-      <c r="L40" s="133"/>
-      <c r="M40" s="133"/>
-      <c r="N40" s="133"/>
-      <c r="O40" s="133"/>
-      <c r="P40" s="133"/>
-      <c r="Q40" s="133"/>
-      <c r="R40" s="133"/>
-      <c r="S40" s="163"/>
-      <c r="T40" s="163"/>
-      <c r="U40" s="163"/>
+      <c r="J40" s="163"/>
+      <c r="K40" s="200"/>
+      <c r="L40" s="201"/>
+      <c r="M40" s="201"/>
+      <c r="N40" s="201"/>
+      <c r="O40" s="201"/>
+      <c r="P40" s="201"/>
+      <c r="Q40" s="201"/>
+      <c r="R40" s="201"/>
+      <c r="S40" s="147"/>
+      <c r="T40" s="147"/>
+      <c r="U40" s="147"/>
     </row>
     <row r="41" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="87" t="s">
+      <c r="A41" s="197" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="177" t="s">
+      <c r="B41" s="198" t="s">
         <v>123</v>
       </c>
       <c r="C41" s="32"/>
@@ -7849,23 +7879,23 @@
       <c r="H41" s="104"/>
       <c r="I41" s="104"/>
       <c r="J41" s="115"/>
-      <c r="K41" s="132"/>
-      <c r="L41" s="133"/>
-      <c r="M41" s="133"/>
-      <c r="N41" s="133"/>
-      <c r="O41" s="133"/>
-      <c r="P41" s="133"/>
-      <c r="Q41" s="163"/>
-      <c r="R41" s="163"/>
-      <c r="S41" s="163"/>
-      <c r="T41" s="163"/>
-      <c r="U41" s="163"/>
+      <c r="K41" s="200"/>
+      <c r="L41" s="201"/>
+      <c r="M41" s="201"/>
+      <c r="N41" s="201"/>
+      <c r="O41" s="201"/>
+      <c r="P41" s="201"/>
+      <c r="Q41" s="147"/>
+      <c r="R41" s="147"/>
+      <c r="S41" s="147"/>
+      <c r="T41" s="147"/>
+      <c r="U41" s="147"/>
     </row>
     <row r="42" spans="1:21" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="87" t="s">
+      <c r="A42" s="197" t="s">
         <v>124</v>
       </c>
-      <c r="B42" s="176" t="s">
+      <c r="B42" s="199" t="s">
         <v>140</v>
       </c>
       <c r="C42" s="32"/>
@@ -7882,23 +7912,23 @@
       <c r="H42" s="104"/>
       <c r="I42" s="104"/>
       <c r="J42" s="115"/>
-      <c r="K42" s="164"/>
-      <c r="L42" s="163"/>
-      <c r="M42" s="133"/>
-      <c r="N42" s="133"/>
-      <c r="O42" s="133"/>
-      <c r="P42" s="133"/>
-      <c r="Q42" s="133"/>
-      <c r="R42" s="133"/>
-      <c r="S42" s="133"/>
-      <c r="T42" s="133"/>
-      <c r="U42" s="133"/>
+      <c r="K42" s="148"/>
+      <c r="L42" s="147"/>
+      <c r="M42" s="201"/>
+      <c r="N42" s="201"/>
+      <c r="O42" s="201"/>
+      <c r="P42" s="201"/>
+      <c r="Q42" s="201"/>
+      <c r="R42" s="201"/>
+      <c r="S42" s="201"/>
+      <c r="T42" s="201"/>
+      <c r="U42" s="201"/>
     </row>
     <row r="43" spans="1:21" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="87" t="s">
+      <c r="A43" s="197" t="s">
         <v>126</v>
       </c>
-      <c r="B43" s="176" t="s">
+      <c r="B43" s="199" t="s">
         <v>139</v>
       </c>
       <c r="C43" s="32"/>
@@ -7909,23 +7939,23 @@
       <c r="H43" s="104"/>
       <c r="I43" s="104"/>
       <c r="J43" s="115"/>
-      <c r="K43" s="164"/>
-      <c r="L43" s="163"/>
-      <c r="M43" s="133"/>
-      <c r="N43" s="133"/>
-      <c r="O43" s="133"/>
-      <c r="P43" s="133"/>
-      <c r="Q43" s="133"/>
-      <c r="R43" s="133"/>
-      <c r="S43" s="133"/>
-      <c r="T43" s="133"/>
-      <c r="U43" s="133"/>
+      <c r="K43" s="148"/>
+      <c r="L43" s="147"/>
+      <c r="M43" s="201"/>
+      <c r="N43" s="201"/>
+      <c r="O43" s="201"/>
+      <c r="P43" s="201"/>
+      <c r="Q43" s="201"/>
+      <c r="R43" s="201"/>
+      <c r="S43" s="201"/>
+      <c r="T43" s="201"/>
+      <c r="U43" s="201"/>
     </row>
     <row r="44" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="87" t="s">
+      <c r="A44" s="197" t="s">
         <v>127</v>
       </c>
-      <c r="B44" s="177" t="s">
+      <c r="B44" s="198" t="s">
         <v>128</v>
       </c>
       <c r="C44" s="32"/>
@@ -7936,23 +7966,23 @@
       <c r="H44" s="104"/>
       <c r="I44" s="104"/>
       <c r="J44" s="115"/>
-      <c r="K44" s="132"/>
-      <c r="L44" s="133"/>
-      <c r="M44" s="133"/>
-      <c r="N44" s="133"/>
-      <c r="O44" s="133"/>
-      <c r="P44" s="163"/>
-      <c r="Q44" s="163"/>
-      <c r="R44" s="163"/>
-      <c r="S44" s="163"/>
-      <c r="T44" s="163"/>
-      <c r="U44" s="163"/>
+      <c r="K44" s="201"/>
+      <c r="L44" s="201"/>
+      <c r="M44" s="201"/>
+      <c r="N44" s="201"/>
+      <c r="O44" s="201"/>
+      <c r="P44" s="147"/>
+      <c r="Q44" s="147"/>
+      <c r="R44" s="147"/>
+      <c r="S44" s="147"/>
+      <c r="T44" s="147"/>
+      <c r="U44" s="147"/>
     </row>
     <row r="45" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="87" t="s">
+      <c r="A45" s="197" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="177" t="s">
+      <c r="B45" s="198" t="s">
         <v>128</v>
       </c>
       <c r="C45" s="32"/>
@@ -7969,23 +7999,23 @@
       <c r="H45" s="104"/>
       <c r="I45" s="104"/>
       <c r="J45" s="115"/>
-      <c r="K45" s="164"/>
-      <c r="L45" s="163"/>
-      <c r="M45" s="163"/>
-      <c r="N45" s="163"/>
-      <c r="O45" s="163"/>
-      <c r="P45" s="163"/>
-      <c r="Q45" s="163"/>
-      <c r="R45" s="163"/>
-      <c r="S45" s="133"/>
-      <c r="T45" s="133"/>
-      <c r="U45" s="133"/>
+      <c r="K45" s="148"/>
+      <c r="L45" s="147"/>
+      <c r="M45" s="147"/>
+      <c r="N45" s="147"/>
+      <c r="O45" s="147"/>
+      <c r="P45" s="147"/>
+      <c r="Q45" s="147"/>
+      <c r="R45" s="147"/>
+      <c r="S45" s="201"/>
+      <c r="T45" s="201"/>
+      <c r="U45" s="201"/>
     </row>
     <row r="46" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="87" t="s">
+      <c r="A46" s="197" t="s">
         <v>136</v>
       </c>
-      <c r="B46" s="177" t="s">
+      <c r="B46" s="198" t="s">
         <v>128</v>
       </c>
       <c r="C46" s="32"/>
@@ -8002,23 +8032,23 @@
       <c r="H46" s="104"/>
       <c r="I46" s="104"/>
       <c r="J46" s="115"/>
-      <c r="K46" s="164"/>
-      <c r="L46" s="163"/>
-      <c r="M46" s="163"/>
-      <c r="N46" s="163"/>
-      <c r="O46" s="133"/>
-      <c r="P46" s="133"/>
-      <c r="Q46" s="133"/>
-      <c r="R46" s="133"/>
-      <c r="S46" s="133"/>
-      <c r="T46" s="133"/>
-      <c r="U46" s="133"/>
+      <c r="K46" s="148"/>
+      <c r="L46" s="147"/>
+      <c r="M46" s="147"/>
+      <c r="N46" s="147"/>
+      <c r="O46" s="201"/>
+      <c r="P46" s="201"/>
+      <c r="Q46" s="201"/>
+      <c r="R46" s="201"/>
+      <c r="S46" s="201"/>
+      <c r="T46" s="201"/>
+      <c r="U46" s="201"/>
     </row>
     <row r="47" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="87" t="s">
+      <c r="A47" s="197" t="s">
         <v>129</v>
       </c>
-      <c r="B47" s="177" t="s">
+      <c r="B47" s="198" t="s">
         <v>125</v>
       </c>
       <c r="C47" s="32"/>
@@ -8035,17 +8065,17 @@
       <c r="H47" s="104"/>
       <c r="I47" s="104"/>
       <c r="J47" s="115"/>
-      <c r="K47" s="132"/>
-      <c r="L47" s="133"/>
-      <c r="M47" s="133"/>
-      <c r="N47" s="133"/>
-      <c r="O47" s="133"/>
-      <c r="P47" s="133"/>
-      <c r="Q47" s="133"/>
-      <c r="R47" s="163"/>
-      <c r="S47" s="163"/>
-      <c r="T47" s="163"/>
-      <c r="U47" s="163"/>
+      <c r="K47" s="201"/>
+      <c r="L47" s="201"/>
+      <c r="M47" s="201"/>
+      <c r="N47" s="201"/>
+      <c r="O47" s="201"/>
+      <c r="P47" s="201"/>
+      <c r="Q47" s="201"/>
+      <c r="R47" s="147"/>
+      <c r="S47" s="147"/>
+      <c r="T47" s="147"/>
+      <c r="U47" s="147"/>
     </row>
     <row r="48" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="33" t="s">
@@ -8076,7 +8106,7 @@
       <c r="A49" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="B49" s="178" t="s">
+      <c r="B49" s="160" t="s">
         <v>132</v>
       </c>
       <c r="C49" s="37"/>
@@ -8097,17 +8127,17 @@
       <c r="N49" s="104"/>
       <c r="O49" s="104"/>
       <c r="P49" s="104"/>
-      <c r="Q49" s="163"/>
-      <c r="R49" s="163"/>
-      <c r="S49" s="163"/>
-      <c r="T49" s="131"/>
-      <c r="U49" s="131"/>
+      <c r="Q49" s="147"/>
+      <c r="R49" s="147"/>
+      <c r="S49" s="147"/>
+      <c r="T49" s="119"/>
+      <c r="U49" s="119"/>
     </row>
     <row r="50" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="B50" s="178" t="s">
+      <c r="B50" s="160" t="s">
         <v>132</v>
       </c>
       <c r="C50" s="37"/>
@@ -8128,17 +8158,17 @@
       <c r="N50" s="104"/>
       <c r="O50" s="104"/>
       <c r="P50" s="104"/>
-      <c r="Q50" s="163"/>
-      <c r="R50" s="163"/>
-      <c r="S50" s="163"/>
-      <c r="T50" s="131"/>
-      <c r="U50" s="131"/>
+      <c r="Q50" s="147"/>
+      <c r="R50" s="147"/>
+      <c r="S50" s="147"/>
+      <c r="T50" s="119"/>
+      <c r="U50" s="119"/>
     </row>
     <row r="51" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="B51" s="178" t="s">
+      <c r="B51" s="160" t="s">
         <v>135</v>
       </c>
       <c r="C51" s="37"/>
@@ -8159,17 +8189,17 @@
       <c r="N51" s="104"/>
       <c r="O51" s="104"/>
       <c r="P51" s="104"/>
-      <c r="Q51" s="163"/>
-      <c r="R51" s="163"/>
-      <c r="S51" s="163"/>
-      <c r="T51" s="131"/>
-      <c r="U51" s="131"/>
+      <c r="Q51" s="147"/>
+      <c r="R51" s="147"/>
+      <c r="S51" s="147"/>
+      <c r="T51" s="119"/>
+      <c r="U51" s="119"/>
     </row>
     <row r="52" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="195" t="s">
+      <c r="A52" s="175" t="s">
         <v>141</v>
       </c>
-      <c r="B52" s="178" t="s">
+      <c r="B52" s="160" t="s">
         <v>115</v>
       </c>
       <c r="C52" s="37"/>
@@ -8190,11 +8220,11 @@
       <c r="N52" s="104"/>
       <c r="O52" s="104"/>
       <c r="P52" s="104"/>
-      <c r="Q52" s="163"/>
-      <c r="R52" s="163"/>
-      <c r="S52" s="163"/>
-      <c r="T52" s="131"/>
-      <c r="U52" s="131"/>
+      <c r="Q52" s="147"/>
+      <c r="R52" s="147"/>
+      <c r="S52" s="147"/>
+      <c r="T52" s="119"/>
+      <c r="U52" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>